<commit_message>
Se corrigieron algunos enlaces
</commit_message>
<xml_diff>
--- a/Imagen Pistas.xlsx
+++ b/Imagen Pistas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\puerc\OneDrive\Documentos\Eric\UNI\Semestre 8\Análisis de Datos\projects\f1\Formula-1-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80D70390-A1D1-44D7-9E77-BE2C58282DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA450ED-D2FD-40EA-9BFD-14FF76A6A440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13005" yWindow="2190" windowWidth="38700" windowHeight="18795" xr2:uid="{E5EC25E1-154B-4B5C-A0FD-B9D6602DDAA4}"/>
+    <workbookView xWindow="9180" yWindow="1890" windowWidth="38700" windowHeight="18795" xr2:uid="{E5EC25E1-154B-4B5C-A0FD-B9D6602DDAA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1128,7 +1128,7 @@
   <dimension ref="A1:I256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="I2" sqref="I2:I256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,11 +1188,11 @@
         <v>11</v>
       </c>
       <c r="H2" t="str">
-        <f>VLOOKUP(B2,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B2,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0a/Albert_Park_Circuit_2021.svg/220px-Albert_Park_Circuit_2021.svg.png</v>
       </c>
       <c r="I2" t="str">
-        <f>VLOOKUP(B2,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B2,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8e/Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -1219,11 +1219,11 @@
         <v>16</v>
       </c>
       <c r="H3" t="str">
-        <f>VLOOKUP(B3,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B3,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/en/thumb/d/d1/Bahrain_International_Circuit_logo.png/200px-Bahrain_International_Circuit_logo.png</v>
       </c>
       <c r="I3" t="str">
-        <f>VLOOKUP(B3,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B3,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bc/Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg/220px-Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -1250,11 +1250,11 @@
         <v>21</v>
       </c>
       <c r="H4" t="str">
-        <f>VLOOKUP(B4,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B4,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/87/Circuit_de_Catalunya_moto_2021.svg/250px-Circuit_de_Catalunya_moto_2021.svg.png</v>
       </c>
       <c r="I4" t="str">
-        <f>VLOOKUP(B4,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B4,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e7/Circuit_de_Barcelona-Catalunya%2C_April_19%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Barcelona-Catalunya%2C_April_19%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -1281,11 +1281,11 @@
         <v>26</v>
       </c>
       <c r="H5" t="str">
-        <f>VLOOKUP(B5,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B5,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e5/Hockenheim2012.svg/220px-Hockenheim2012.svg.png</v>
       </c>
       <c r="I5" t="str">
-        <f>VLOOKUP(B5,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B5,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/41/Hockenheimring%2C_April_29%2C_2018_SkySat_%28crop%29.jpg/220px-Hockenheimring%2C_April_29%2C_2018_SkySat_%28crop%29.jpg</v>
       </c>
     </row>
@@ -1312,11 +1312,11 @@
         <v>31</v>
       </c>
       <c r="H6" t="str">
-        <f>VLOOKUP(B6,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B6,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/91/Hungaroring.svg/260px-Hungaroring.svg.png</v>
       </c>
       <c r="I6" t="str">
-        <f>VLOOKUP(B6,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B6,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/a/aa/Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg/220px-Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -1343,11 +1343,11 @@
         <v>36</v>
       </c>
       <c r="H7" t="str">
-        <f>VLOOKUP(B7,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B7,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/cf/Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace_%28AKA_Interlagos%29_track_map.svg/260px-Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace_%28AKA_Interlagos%29_track_map.svg.png</v>
       </c>
       <c r="I7" t="str">
-        <f>VLOOKUP(B7,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B7,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/70/Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace%2C_July_3%2C_2018_SkySat_%28cropped%29.jpg/220px-Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace%2C_July_3%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -1374,11 +1374,11 @@
         <v>41</v>
       </c>
       <c r="H8" t="str">
-        <f>VLOOKUP(B8,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B8,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/en/7/7c/Istanbulpark.png</v>
       </c>
       <c r="I8" t="str">
-        <f>VLOOKUP(B8,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B8,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/90/Istanbul_Park_aerial.jpg/270px-Istanbul_Park_aerial.jpg</v>
       </c>
     </row>
@@ -1405,11 +1405,11 @@
         <v>46</v>
       </c>
       <c r="H9" t="str">
-        <f>VLOOKUP(B9,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B9,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/17/Planned_2023_Marina_Bay_Street_Circuit_layout.png/220px-Planned_2023_Marina_Bay_Street_Circuit_layout.png</v>
       </c>
       <c r="I9" t="str">
-        <f>VLOOKUP(B9,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B9,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f0/1_singapore_f1_night_race_2012_city_skyline.jpg/240px-1_singapore_f1_night_race_2012_city_skyline.jpg</v>
       </c>
     </row>
@@ -1436,11 +1436,11 @@
         <v>51</v>
       </c>
       <c r="H10" t="str">
-        <f>VLOOKUP(B10,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B10,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/3/36/Monte_Carlo_Formula_1_track_map.svg/250px-Monte_Carlo_Formula_1_track_map.svg.png</v>
       </c>
       <c r="I10" t="str">
-        <f>VLOOKUP(B10,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B10,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/c7/Circuit_de_Monaco%2C_April_1%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Monaco%2C_April_1%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -1467,11 +1467,11 @@
         <v>56</v>
       </c>
       <c r="H11" t="str">
-        <f>VLOOKUP(B11,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B11,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
       </c>
       <c r="I11" t="str">
-        <f>VLOOKUP(B11,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B11,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -1498,11 +1498,11 @@
         <v>61</v>
       </c>
       <c r="H12" t="str">
-        <f>VLOOKUP(B12,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B12,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/67/Sepang.svg/250px-Sepang.svg.png</v>
       </c>
       <c r="I12" t="str">
-        <f>VLOOKUP(B12,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B12,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/7f/Sepang_International_Circuit_1.JPG/220px-Sepang_International_Circuit_1.JPG</v>
       </c>
     </row>
@@ -1529,11 +1529,11 @@
         <v>66</v>
       </c>
       <c r="H13" t="str">
-        <f>VLOOKUP(B13,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B13,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/14/Shanghai_International_Racing_Circuit_track_map.svg/250px-Shanghai_International_Racing_Circuit_track_map.svg.png</v>
       </c>
       <c r="I13" t="str">
-        <f>VLOOKUP(B13,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B13,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/d/d6/Shanghai_International_Circuit%2C_April_7%2C_2018_SkySat_%28rotated%29.jpg/220px-Shanghai_International_Circuit%2C_April_7%2C_2018_SkySat_%28rotated%29.jpg</v>
       </c>
     </row>
@@ -1560,11 +1560,11 @@
         <v>71</v>
       </c>
       <c r="H14" t="str">
-        <f>VLOOKUP(B14,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B14,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bd/Silverstone_Circuit_2020.png/250px-Silverstone_Circuit_2020.png</v>
       </c>
       <c r="I14" t="str">
-        <f>VLOOKUP(B14,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B14,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8d/Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg/220px-Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -1591,11 +1591,11 @@
         <v>76</v>
       </c>
       <c r="H15" t="str">
-        <f>VLOOKUP(B15,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B15,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/5/54/Spa-Francorchamps_of_Belgium.svg/260px-Spa-Francorchamps_of_Belgium.svg.png</v>
       </c>
       <c r="I15" t="str">
-        <f>VLOOKUP(B15,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B15,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/77/Circuit_de_Spa-Francorchamps%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Spa-Francorchamps%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -1622,11 +1622,11 @@
         <v>81</v>
       </c>
       <c r="H16" t="str">
-        <f>VLOOKUP(B16,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B16,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/ec/Suzuka_circuit_map--2005.svg/260px-Suzuka_circuit_map--2005.svg.png</v>
       </c>
       <c r="I16" t="str">
-        <f>VLOOKUP(B16,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B16,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/9a/Suzuka_International_Racing_Course%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg/220px-Suzuka_International_Racing_Course%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -1653,11 +1653,11 @@
         <v>85</v>
       </c>
       <c r="H17" t="str">
-        <f>VLOOKUP(B17,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B17,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0e/Circuit_Valensia_street.svg/250px-Circuit_Valensia_street.svg.png</v>
       </c>
       <c r="I17" t="str">
-        <f>VLOOKUP(B17,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B17,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/ff/Swing-bridge_Valencia_Street_Circuit.jpg/220px-Swing-bridge_Valencia_Street_Circuit.jpg</v>
       </c>
     </row>
@@ -1684,11 +1684,11 @@
         <v>90</v>
       </c>
       <c r="H18" t="str">
-        <f>VLOOKUP(B18,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B18,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f9/%C3%8Ele_Notre-Dame_%28Circuit_Gilles_Villeneuve%29.svg/280px-%C3%8Ele_Notre-Dame_%28Circuit_Gilles_Villeneuve%29.svg.png</v>
       </c>
       <c r="I18" t="str">
-        <f>VLOOKUP(B18,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B18,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/3/38/F1_1978_circuit_ile_notre_dame.png/220px-F1_1978_circuit_ile_notre_dame.png</v>
       </c>
     </row>
@@ -1715,12 +1715,12 @@
         <v>95</v>
       </c>
       <c r="H19" t="str">
-        <f>VLOOKUP(B19,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/4c/Losail.svg/250px-Losail.svg.png</v>
+        <f>VLOOKUP(B19,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/b0/Yas_Marina_Circuit.png/250px-Yas_Marina_Circuit.png</v>
       </c>
       <c r="I19" t="str">
-        <f>VLOOKUP(B19,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://www.racefans.net/wp-content/uploads/2021/07/racefansdotnet-21-07-24-21-06-40-1.jpg</v>
+        <f>VLOOKUP(B19,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e1/Yas_Marina_Circuit%2C_October_12%2C_2018_SkySat_%28cropped%29.jpg/220px-Yas_Marina_Circuit%2C_October_12%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1746,12 +1746,12 @@
         <v>100</v>
       </c>
       <c r="H20" t="str">
-        <f>VLOOKUP(B20,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/4c/Losail.svg/250px-Losail.svg.png</v>
+        <f>VLOOKUP(B20,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/2/29/Korea_international_circuit_v3.svg/260px-Korea_international_circuit_v3.svg.png</v>
       </c>
       <c r="I20" t="str">
-        <f>VLOOKUP(B20,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://www.racefans.net/wp-content/uploads/2021/07/racefansdotnet-21-07-24-21-06-40-1.jpg</v>
+        <f>VLOOKUP(B20,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcSb2epC9a8qoZyccNJCgRnRtPYPEDOhbu7C3A&amp;usqp=CAU</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1777,11 +1777,11 @@
         <v>11</v>
       </c>
       <c r="H21" t="str">
-        <f>VLOOKUP(B21,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B21,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0a/Albert_Park_Circuit_2021.svg/220px-Albert_Park_Circuit_2021.svg.png</v>
       </c>
       <c r="I21" t="str">
-        <f>VLOOKUP(B21,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B21,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8e/Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -1808,12 +1808,12 @@
         <v>105</v>
       </c>
       <c r="H22" t="str">
-        <f>VLOOKUP(B22,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/en/thumb/d/d1/Bahrain_International_Circuit_logo.png/200px-Bahrain_International_Circuit_logo.png</v>
+        <f>VLOOKUP(B22,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/2/26/Buddh_Circuit_1.svg/250px-Buddh_Circuit_1.svg.png</v>
       </c>
       <c r="I22" t="str">
-        <f>VLOOKUP(B22,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bc/Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg/220px-Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B22,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/66/Buddh_International_Circuit_aerial.jpg/350px-Buddh_International_Circuit_aerial.jpg</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1839,11 +1839,11 @@
         <v>21</v>
       </c>
       <c r="H23" t="str">
-        <f>VLOOKUP(B23,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B23,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/87/Circuit_de_Catalunya_moto_2021.svg/250px-Circuit_de_Catalunya_moto_2021.svg.png</v>
       </c>
       <c r="I23" t="str">
-        <f>VLOOKUP(B23,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B23,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e7/Circuit_de_Barcelona-Catalunya%2C_April_19%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Barcelona-Catalunya%2C_April_19%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -1870,11 +1870,11 @@
         <v>31</v>
       </c>
       <c r="H24" t="str">
-        <f>VLOOKUP(B24,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B24,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/91/Hungaroring.svg/260px-Hungaroring.svg.png</v>
       </c>
       <c r="I24" t="str">
-        <f>VLOOKUP(B24,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B24,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/a/aa/Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg/220px-Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -1901,11 +1901,11 @@
         <v>36</v>
       </c>
       <c r="H25" t="str">
-        <f>VLOOKUP(B25,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B25,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/cf/Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace_%28AKA_Interlagos%29_track_map.svg/260px-Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace_%28AKA_Interlagos%29_track_map.svg.png</v>
       </c>
       <c r="I25" t="str">
-        <f>VLOOKUP(B25,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B25,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/70/Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace%2C_July_3%2C_2018_SkySat_%28cropped%29.jpg/220px-Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace%2C_July_3%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -1932,11 +1932,11 @@
         <v>41</v>
       </c>
       <c r="H26" t="str">
-        <f>VLOOKUP(B26,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B26,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/en/7/7c/Istanbulpark.png</v>
       </c>
       <c r="I26" t="str">
-        <f>VLOOKUP(B26,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B26,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/90/Istanbul_Park_aerial.jpg/270px-Istanbul_Park_aerial.jpg</v>
       </c>
     </row>
@@ -1963,11 +1963,11 @@
         <v>46</v>
       </c>
       <c r="H27" t="str">
-        <f>VLOOKUP(B27,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B27,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/17/Planned_2023_Marina_Bay_Street_Circuit_layout.png/220px-Planned_2023_Marina_Bay_Street_Circuit_layout.png</v>
       </c>
       <c r="I27" t="str">
-        <f>VLOOKUP(B27,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B27,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f0/1_singapore_f1_night_race_2012_city_skyline.jpg/240px-1_singapore_f1_night_race_2012_city_skyline.jpg</v>
       </c>
     </row>
@@ -1994,11 +1994,11 @@
         <v>51</v>
       </c>
       <c r="H28" t="str">
-        <f>VLOOKUP(B28,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B28,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/3/36/Monte_Carlo_Formula_1_track_map.svg/250px-Monte_Carlo_Formula_1_track_map.svg.png</v>
       </c>
       <c r="I28" t="str">
-        <f>VLOOKUP(B28,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B28,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/c7/Circuit_de_Monaco%2C_April_1%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Monaco%2C_April_1%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -2025,11 +2025,11 @@
         <v>56</v>
       </c>
       <c r="H29" t="str">
-        <f>VLOOKUP(B29,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B29,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
       </c>
       <c r="I29" t="str">
-        <f>VLOOKUP(B29,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B29,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -2056,12 +2056,12 @@
         <v>109</v>
       </c>
       <c r="H30" t="str">
-        <f>VLOOKUP(B30,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
+        <f>VLOOKUP(B30,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/76/N%C3%BCrburgring_-_Grand-Prix-Strecke.svg/230px-N%C3%BCrburgring_-_Grand-Prix-Strecke.svg.png</v>
       </c>
       <c r="I30" t="str">
-        <f>VLOOKUP(B30,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B30,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/4c/Panorama_N%C3%BCrburgring_Haupteingang_2010.jpg/530px-Panorama_N%C3%BCrburgring_Haupteingang_2010.jpg</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -2087,11 +2087,11 @@
         <v>61</v>
       </c>
       <c r="H31" t="str">
-        <f>VLOOKUP(B31,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B31,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/67/Sepang.svg/250px-Sepang.svg.png</v>
       </c>
       <c r="I31" t="str">
-        <f>VLOOKUP(B31,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B31,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/7f/Sepang_International_Circuit_1.JPG/220px-Sepang_International_Circuit_1.JPG</v>
       </c>
     </row>
@@ -2118,11 +2118,11 @@
         <v>66</v>
       </c>
       <c r="H32" t="str">
-        <f>VLOOKUP(B32,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B32,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/14/Shanghai_International_Racing_Circuit_track_map.svg/250px-Shanghai_International_Racing_Circuit_track_map.svg.png</v>
       </c>
       <c r="I32" t="str">
-        <f>VLOOKUP(B32,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B32,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/d/d6/Shanghai_International_Circuit%2C_April_7%2C_2018_SkySat_%28rotated%29.jpg/220px-Shanghai_International_Circuit%2C_April_7%2C_2018_SkySat_%28rotated%29.jpg</v>
       </c>
     </row>
@@ -2149,11 +2149,11 @@
         <v>71</v>
       </c>
       <c r="H33" t="str">
-        <f>VLOOKUP(B33,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B33,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bd/Silverstone_Circuit_2020.png/250px-Silverstone_Circuit_2020.png</v>
       </c>
       <c r="I33" t="str">
-        <f>VLOOKUP(B33,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B33,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8d/Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg/220px-Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -2180,11 +2180,11 @@
         <v>76</v>
       </c>
       <c r="H34" t="str">
-        <f>VLOOKUP(B34,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B34,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/5/54/Spa-Francorchamps_of_Belgium.svg/260px-Spa-Francorchamps_of_Belgium.svg.png</v>
       </c>
       <c r="I34" t="str">
-        <f>VLOOKUP(B34,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B34,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/77/Circuit_de_Spa-Francorchamps%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Spa-Francorchamps%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -2211,11 +2211,11 @@
         <v>81</v>
       </c>
       <c r="H35" t="str">
-        <f>VLOOKUP(B35,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B35,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/ec/Suzuka_circuit_map--2005.svg/260px-Suzuka_circuit_map--2005.svg.png</v>
       </c>
       <c r="I35" t="str">
-        <f>VLOOKUP(B35,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B35,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/9a/Suzuka_International_Racing_Course%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg/220px-Suzuka_International_Racing_Course%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -2242,11 +2242,11 @@
         <v>85</v>
       </c>
       <c r="H36" t="str">
-        <f>VLOOKUP(B36,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B36,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0e/Circuit_Valensia_street.svg/250px-Circuit_Valensia_street.svg.png</v>
       </c>
       <c r="I36" t="str">
-        <f>VLOOKUP(B36,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B36,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/ff/Swing-bridge_Valencia_Street_Circuit.jpg/220px-Swing-bridge_Valencia_Street_Circuit.jpg</v>
       </c>
     </row>
@@ -2273,11 +2273,11 @@
         <v>90</v>
       </c>
       <c r="H37" t="str">
-        <f>VLOOKUP(B37,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B37,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f9/%C3%8Ele_Notre-Dame_%28Circuit_Gilles_Villeneuve%29.svg/280px-%C3%8Ele_Notre-Dame_%28Circuit_Gilles_Villeneuve%29.svg.png</v>
       </c>
       <c r="I37" t="str">
-        <f>VLOOKUP(B37,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B37,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/3/38/F1_1978_circuit_ile_notre_dame.png/220px-F1_1978_circuit_ile_notre_dame.png</v>
       </c>
     </row>
@@ -2304,12 +2304,12 @@
         <v>95</v>
       </c>
       <c r="H38" t="str">
-        <f>VLOOKUP(B38,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/4c/Losail.svg/250px-Losail.svg.png</v>
+        <f>VLOOKUP(B38,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/b0/Yas_Marina_Circuit.png/250px-Yas_Marina_Circuit.png</v>
       </c>
       <c r="I38" t="str">
-        <f>VLOOKUP(B38,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://www.racefans.net/wp-content/uploads/2021/07/racefansdotnet-21-07-24-21-06-40-1.jpg</v>
+        <f>VLOOKUP(B38,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e1/Yas_Marina_Circuit%2C_October_12%2C_2018_SkySat_%28cropped%29.jpg/220px-Yas_Marina_Circuit%2C_October_12%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2335,12 +2335,12 @@
         <v>100</v>
       </c>
       <c r="H39" t="str">
-        <f>VLOOKUP(B39,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/4c/Losail.svg/250px-Losail.svg.png</v>
+        <f>VLOOKUP(B39,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/2/29/Korea_international_circuit_v3.svg/260px-Korea_international_circuit_v3.svg.png</v>
       </c>
       <c r="I39" t="str">
-        <f>VLOOKUP(B39,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://www.racefans.net/wp-content/uploads/2021/07/racefansdotnet-21-07-24-21-06-40-1.jpg</v>
+        <f>VLOOKUP(B39,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcSb2epC9a8qoZyccNJCgRnRtPYPEDOhbu7C3A&amp;usqp=CAU</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2366,11 +2366,11 @@
         <v>11</v>
       </c>
       <c r="H40" t="str">
-        <f>VLOOKUP(B40,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B40,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0a/Albert_Park_Circuit_2021.svg/220px-Albert_Park_Circuit_2021.svg.png</v>
       </c>
       <c r="I40" t="str">
-        <f>VLOOKUP(B40,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B40,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8e/Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -2397,12 +2397,12 @@
         <v>114</v>
       </c>
       <c r="H41" t="str">
-        <f>VLOOKUP(B41,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0a/Albert_Park_Circuit_2021.svg/220px-Albert_Park_Circuit_2021.svg.png</v>
+        <f>VLOOKUP(B41,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/a/a5/Austin_circuit.svg/250px-Austin_circuit.svg.png</v>
       </c>
       <c r="I41" t="str">
-        <f>VLOOKUP(B41,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8e/Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B41,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/78/Circuit_of_the_Americas%2C_April_22%2C_2018_SkySat_%28cropped2%29.jpg/220px-Circuit_of_the_Americas%2C_April_22%2C_2018_SkySat_%28cropped2%29.jpg</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -2428,11 +2428,11 @@
         <v>16</v>
       </c>
       <c r="H42" t="str">
-        <f>VLOOKUP(B42,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B42,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/en/thumb/d/d1/Bahrain_International_Circuit_logo.png/200px-Bahrain_International_Circuit_logo.png</v>
       </c>
       <c r="I42" t="str">
-        <f>VLOOKUP(B42,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B42,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bc/Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg/220px-Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -2459,12 +2459,12 @@
         <v>105</v>
       </c>
       <c r="H43" t="str">
-        <f>VLOOKUP(B43,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/en/thumb/d/d1/Bahrain_International_Circuit_logo.png/200px-Bahrain_International_Circuit_logo.png</v>
+        <f>VLOOKUP(B43,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/2/26/Buddh_Circuit_1.svg/250px-Buddh_Circuit_1.svg.png</v>
       </c>
       <c r="I43" t="str">
-        <f>VLOOKUP(B43,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bc/Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg/220px-Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B43,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/66/Buddh_International_Circuit_aerial.jpg/350px-Buddh_International_Circuit_aerial.jpg</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -2490,11 +2490,11 @@
         <v>21</v>
       </c>
       <c r="H44" t="str">
-        <f>VLOOKUP(B44,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B44,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/87/Circuit_de_Catalunya_moto_2021.svg/250px-Circuit_de_Catalunya_moto_2021.svg.png</v>
       </c>
       <c r="I44" t="str">
-        <f>VLOOKUP(B44,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B44,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e7/Circuit_de_Barcelona-Catalunya%2C_April_19%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Barcelona-Catalunya%2C_April_19%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -2521,11 +2521,11 @@
         <v>26</v>
       </c>
       <c r="H45" t="str">
-        <f>VLOOKUP(B45,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B45,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e5/Hockenheim2012.svg/220px-Hockenheim2012.svg.png</v>
       </c>
       <c r="I45" t="str">
-        <f>VLOOKUP(B45,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B45,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/41/Hockenheimring%2C_April_29%2C_2018_SkySat_%28crop%29.jpg/220px-Hockenheimring%2C_April_29%2C_2018_SkySat_%28crop%29.jpg</v>
       </c>
     </row>
@@ -2552,11 +2552,11 @@
         <v>31</v>
       </c>
       <c r="H46" t="str">
-        <f>VLOOKUP(B46,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B46,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/91/Hungaroring.svg/260px-Hungaroring.svg.png</v>
       </c>
       <c r="I46" t="str">
-        <f>VLOOKUP(B46,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B46,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/a/aa/Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg/220px-Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -2583,11 +2583,11 @@
         <v>36</v>
       </c>
       <c r="H47" t="str">
-        <f>VLOOKUP(B47,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B47,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/cf/Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace_%28AKA_Interlagos%29_track_map.svg/260px-Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace_%28AKA_Interlagos%29_track_map.svg.png</v>
       </c>
       <c r="I47" t="str">
-        <f>VLOOKUP(B47,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B47,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/70/Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace%2C_July_3%2C_2018_SkySat_%28cropped%29.jpg/220px-Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace%2C_July_3%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -2614,11 +2614,11 @@
         <v>46</v>
       </c>
       <c r="H48" t="str">
-        <f>VLOOKUP(B48,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B48,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/17/Planned_2023_Marina_Bay_Street_Circuit_layout.png/220px-Planned_2023_Marina_Bay_Street_Circuit_layout.png</v>
       </c>
       <c r="I48" t="str">
-        <f>VLOOKUP(B48,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B48,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f0/1_singapore_f1_night_race_2012_city_skyline.jpg/240px-1_singapore_f1_night_race_2012_city_skyline.jpg</v>
       </c>
     </row>
@@ -2645,11 +2645,11 @@
         <v>51</v>
       </c>
       <c r="H49" t="str">
-        <f>VLOOKUP(B49,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B49,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/3/36/Monte_Carlo_Formula_1_track_map.svg/250px-Monte_Carlo_Formula_1_track_map.svg.png</v>
       </c>
       <c r="I49" t="str">
-        <f>VLOOKUP(B49,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B49,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/c7/Circuit_de_Monaco%2C_April_1%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Monaco%2C_April_1%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -2676,11 +2676,11 @@
         <v>56</v>
       </c>
       <c r="H50" t="str">
-        <f>VLOOKUP(B50,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B50,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
       </c>
       <c r="I50" t="str">
-        <f>VLOOKUP(B50,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B50,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -2707,11 +2707,11 @@
         <v>61</v>
       </c>
       <c r="H51" t="str">
-        <f>VLOOKUP(B51,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B51,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/67/Sepang.svg/250px-Sepang.svg.png</v>
       </c>
       <c r="I51" t="str">
-        <f>VLOOKUP(B51,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B51,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/7f/Sepang_International_Circuit_1.JPG/220px-Sepang_International_Circuit_1.JPG</v>
       </c>
     </row>
@@ -2738,11 +2738,11 @@
         <v>66</v>
       </c>
       <c r="H52" t="str">
-        <f>VLOOKUP(B52,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B52,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/14/Shanghai_International_Racing_Circuit_track_map.svg/250px-Shanghai_International_Racing_Circuit_track_map.svg.png</v>
       </c>
       <c r="I52" t="str">
-        <f>VLOOKUP(B52,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B52,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/d/d6/Shanghai_International_Circuit%2C_April_7%2C_2018_SkySat_%28rotated%29.jpg/220px-Shanghai_International_Circuit%2C_April_7%2C_2018_SkySat_%28rotated%29.jpg</v>
       </c>
     </row>
@@ -2769,11 +2769,11 @@
         <v>71</v>
       </c>
       <c r="H53" t="str">
-        <f>VLOOKUP(B53,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B53,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bd/Silverstone_Circuit_2020.png/250px-Silverstone_Circuit_2020.png</v>
       </c>
       <c r="I53" t="str">
-        <f>VLOOKUP(B53,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B53,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8d/Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg/220px-Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -2800,11 +2800,11 @@
         <v>76</v>
       </c>
       <c r="H54" t="str">
-        <f>VLOOKUP(B54,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B54,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/5/54/Spa-Francorchamps_of_Belgium.svg/260px-Spa-Francorchamps_of_Belgium.svg.png</v>
       </c>
       <c r="I54" t="str">
-        <f>VLOOKUP(B54,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B54,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/77/Circuit_de_Spa-Francorchamps%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Spa-Francorchamps%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -2831,11 +2831,11 @@
         <v>81</v>
       </c>
       <c r="H55" t="str">
-        <f>VLOOKUP(B55,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B55,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/ec/Suzuka_circuit_map--2005.svg/260px-Suzuka_circuit_map--2005.svg.png</v>
       </c>
       <c r="I55" t="str">
-        <f>VLOOKUP(B55,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B55,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/9a/Suzuka_International_Racing_Course%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg/220px-Suzuka_International_Racing_Course%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -2862,11 +2862,11 @@
         <v>85</v>
       </c>
       <c r="H56" t="str">
-        <f>VLOOKUP(B56,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B56,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0e/Circuit_Valensia_street.svg/250px-Circuit_Valensia_street.svg.png</v>
       </c>
       <c r="I56" t="str">
-        <f>VLOOKUP(B56,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B56,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/ff/Swing-bridge_Valencia_Street_Circuit.jpg/220px-Swing-bridge_Valencia_Street_Circuit.jpg</v>
       </c>
     </row>
@@ -2893,11 +2893,11 @@
         <v>90</v>
       </c>
       <c r="H57" t="str">
-        <f>VLOOKUP(B57,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B57,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f9/%C3%8Ele_Notre-Dame_%28Circuit_Gilles_Villeneuve%29.svg/280px-%C3%8Ele_Notre-Dame_%28Circuit_Gilles_Villeneuve%29.svg.png</v>
       </c>
       <c r="I57" t="str">
-        <f>VLOOKUP(B57,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B57,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/3/38/F1_1978_circuit_ile_notre_dame.png/220px-F1_1978_circuit_ile_notre_dame.png</v>
       </c>
     </row>
@@ -2924,12 +2924,12 @@
         <v>95</v>
       </c>
       <c r="H58" t="str">
-        <f>VLOOKUP(B58,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/4c/Losail.svg/250px-Losail.svg.png</v>
+        <f>VLOOKUP(B58,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/b0/Yas_Marina_Circuit.png/250px-Yas_Marina_Circuit.png</v>
       </c>
       <c r="I58" t="str">
-        <f>VLOOKUP(B58,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://www.racefans.net/wp-content/uploads/2021/07/racefansdotnet-21-07-24-21-06-40-1.jpg</v>
+        <f>VLOOKUP(B58,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e1/Yas_Marina_Circuit%2C_October_12%2C_2018_SkySat_%28cropped%29.jpg/220px-Yas_Marina_Circuit%2C_October_12%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -2955,12 +2955,12 @@
         <v>100</v>
       </c>
       <c r="H59" t="str">
-        <f>VLOOKUP(B59,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/4c/Losail.svg/250px-Losail.svg.png</v>
+        <f>VLOOKUP(B59,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/2/29/Korea_international_circuit_v3.svg/260px-Korea_international_circuit_v3.svg.png</v>
       </c>
       <c r="I59" t="str">
-        <f>VLOOKUP(B59,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://www.racefans.net/wp-content/uploads/2021/07/racefansdotnet-21-07-24-21-06-40-1.jpg</v>
+        <f>VLOOKUP(B59,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcSb2epC9a8qoZyccNJCgRnRtPYPEDOhbu7C3A&amp;usqp=CAU</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -2986,11 +2986,11 @@
         <v>11</v>
       </c>
       <c r="H60" t="str">
-        <f>VLOOKUP(B60,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B60,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0a/Albert_Park_Circuit_2021.svg/220px-Albert_Park_Circuit_2021.svg.png</v>
       </c>
       <c r="I60" t="str">
-        <f>VLOOKUP(B60,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B60,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8e/Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -3017,12 +3017,12 @@
         <v>114</v>
       </c>
       <c r="H61" t="str">
-        <f>VLOOKUP(B61,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0a/Albert_Park_Circuit_2021.svg/220px-Albert_Park_Circuit_2021.svg.png</v>
+        <f>VLOOKUP(B61,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/a/a5/Austin_circuit.svg/250px-Austin_circuit.svg.png</v>
       </c>
       <c r="I61" t="str">
-        <f>VLOOKUP(B61,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8e/Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B61,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/78/Circuit_of_the_Americas%2C_April_22%2C_2018_SkySat_%28cropped2%29.jpg/220px-Circuit_of_the_Americas%2C_April_22%2C_2018_SkySat_%28cropped2%29.jpg</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -3048,11 +3048,11 @@
         <v>16</v>
       </c>
       <c r="H62" t="str">
-        <f>VLOOKUP(B62,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B62,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/en/thumb/d/d1/Bahrain_International_Circuit_logo.png/200px-Bahrain_International_Circuit_logo.png</v>
       </c>
       <c r="I62" t="str">
-        <f>VLOOKUP(B62,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B62,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bc/Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg/220px-Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -3079,12 +3079,12 @@
         <v>105</v>
       </c>
       <c r="H63" t="str">
-        <f>VLOOKUP(B63,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/en/thumb/d/d1/Bahrain_International_Circuit_logo.png/200px-Bahrain_International_Circuit_logo.png</v>
+        <f>VLOOKUP(B63,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/2/26/Buddh_Circuit_1.svg/250px-Buddh_Circuit_1.svg.png</v>
       </c>
       <c r="I63" t="str">
-        <f>VLOOKUP(B63,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bc/Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg/220px-Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B63,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/66/Buddh_International_Circuit_aerial.jpg/350px-Buddh_International_Circuit_aerial.jpg</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -3110,11 +3110,11 @@
         <v>21</v>
       </c>
       <c r="H64" t="str">
-        <f>VLOOKUP(B64,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B64,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/87/Circuit_de_Catalunya_moto_2021.svg/250px-Circuit_de_Catalunya_moto_2021.svg.png</v>
       </c>
       <c r="I64" t="str">
-        <f>VLOOKUP(B64,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B64,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e7/Circuit_de_Barcelona-Catalunya%2C_April_19%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Barcelona-Catalunya%2C_April_19%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -3141,11 +3141,11 @@
         <v>31</v>
       </c>
       <c r="H65" t="str">
-        <f>VLOOKUP(B65,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B65,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/91/Hungaroring.svg/260px-Hungaroring.svg.png</v>
       </c>
       <c r="I65" t="str">
-        <f>VLOOKUP(B65,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B65,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/a/aa/Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg/220px-Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -3172,11 +3172,11 @@
         <v>36</v>
       </c>
       <c r="H66" t="str">
-        <f>VLOOKUP(B66,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B66,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/cf/Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace_%28AKA_Interlagos%29_track_map.svg/260px-Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace_%28AKA_Interlagos%29_track_map.svg.png</v>
       </c>
       <c r="I66" t="str">
-        <f>VLOOKUP(B66,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B66,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/70/Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace%2C_July_3%2C_2018_SkySat_%28cropped%29.jpg/220px-Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace%2C_July_3%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -3203,11 +3203,11 @@
         <v>46</v>
       </c>
       <c r="H67" t="str">
-        <f>VLOOKUP(B67,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B67,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/17/Planned_2023_Marina_Bay_Street_Circuit_layout.png/220px-Planned_2023_Marina_Bay_Street_Circuit_layout.png</v>
       </c>
       <c r="I67" t="str">
-        <f>VLOOKUP(B67,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B67,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f0/1_singapore_f1_night_race_2012_city_skyline.jpg/240px-1_singapore_f1_night_race_2012_city_skyline.jpg</v>
       </c>
     </row>
@@ -3234,11 +3234,11 @@
         <v>51</v>
       </c>
       <c r="H68" t="str">
-        <f>VLOOKUP(B68,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B68,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/3/36/Monte_Carlo_Formula_1_track_map.svg/250px-Monte_Carlo_Formula_1_track_map.svg.png</v>
       </c>
       <c r="I68" t="str">
-        <f>VLOOKUP(B68,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B68,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/c7/Circuit_de_Monaco%2C_April_1%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Monaco%2C_April_1%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -3265,11 +3265,11 @@
         <v>56</v>
       </c>
       <c r="H69" t="str">
-        <f>VLOOKUP(B69,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B69,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
       </c>
       <c r="I69" t="str">
-        <f>VLOOKUP(B69,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B69,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -3296,12 +3296,12 @@
         <v>109</v>
       </c>
       <c r="H70" t="str">
-        <f>VLOOKUP(B70,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
+        <f>VLOOKUP(B70,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/76/N%C3%BCrburgring_-_Grand-Prix-Strecke.svg/230px-N%C3%BCrburgring_-_Grand-Prix-Strecke.svg.png</v>
       </c>
       <c r="I70" t="str">
-        <f>VLOOKUP(B70,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B70,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/4c/Panorama_N%C3%BCrburgring_Haupteingang_2010.jpg/530px-Panorama_N%C3%BCrburgring_Haupteingang_2010.jpg</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -3327,11 +3327,11 @@
         <v>61</v>
       </c>
       <c r="H71" t="str">
-        <f>VLOOKUP(B71,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B71,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/67/Sepang.svg/250px-Sepang.svg.png</v>
       </c>
       <c r="I71" t="str">
-        <f>VLOOKUP(B71,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B71,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/7f/Sepang_International_Circuit_1.JPG/220px-Sepang_International_Circuit_1.JPG</v>
       </c>
     </row>
@@ -3358,11 +3358,11 @@
         <v>66</v>
       </c>
       <c r="H72" t="str">
-        <f>VLOOKUP(B72,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B72,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/14/Shanghai_International_Racing_Circuit_track_map.svg/250px-Shanghai_International_Racing_Circuit_track_map.svg.png</v>
       </c>
       <c r="I72" t="str">
-        <f>VLOOKUP(B72,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B72,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/d/d6/Shanghai_International_Circuit%2C_April_7%2C_2018_SkySat_%28rotated%29.jpg/220px-Shanghai_International_Circuit%2C_April_7%2C_2018_SkySat_%28rotated%29.jpg</v>
       </c>
     </row>
@@ -3389,11 +3389,11 @@
         <v>71</v>
       </c>
       <c r="H73" t="str">
-        <f>VLOOKUP(B73,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B73,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bd/Silverstone_Circuit_2020.png/250px-Silverstone_Circuit_2020.png</v>
       </c>
       <c r="I73" t="str">
-        <f>VLOOKUP(B73,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B73,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8d/Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg/220px-Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -3420,11 +3420,11 @@
         <v>76</v>
       </c>
       <c r="H74" t="str">
-        <f>VLOOKUP(B74,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B74,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/5/54/Spa-Francorchamps_of_Belgium.svg/260px-Spa-Francorchamps_of_Belgium.svg.png</v>
       </c>
       <c r="I74" t="str">
-        <f>VLOOKUP(B74,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B74,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/77/Circuit_de_Spa-Francorchamps%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Spa-Francorchamps%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -3451,11 +3451,11 @@
         <v>81</v>
       </c>
       <c r="H75" t="str">
-        <f>VLOOKUP(B75,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B75,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/ec/Suzuka_circuit_map--2005.svg/260px-Suzuka_circuit_map--2005.svg.png</v>
       </c>
       <c r="I75" t="str">
-        <f>VLOOKUP(B75,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B75,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/9a/Suzuka_International_Racing_Course%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg/220px-Suzuka_International_Racing_Course%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -3482,11 +3482,11 @@
         <v>90</v>
       </c>
       <c r="H76" t="str">
-        <f>VLOOKUP(B76,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B76,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f9/%C3%8Ele_Notre-Dame_%28Circuit_Gilles_Villeneuve%29.svg/280px-%C3%8Ele_Notre-Dame_%28Circuit_Gilles_Villeneuve%29.svg.png</v>
       </c>
       <c r="I76" t="str">
-        <f>VLOOKUP(B76,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B76,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/3/38/F1_1978_circuit_ile_notre_dame.png/220px-F1_1978_circuit_ile_notre_dame.png</v>
       </c>
     </row>
@@ -3513,12 +3513,12 @@
         <v>95</v>
       </c>
       <c r="H77" t="str">
-        <f>VLOOKUP(B77,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/4c/Losail.svg/250px-Losail.svg.png</v>
+        <f>VLOOKUP(B77,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/b0/Yas_Marina_Circuit.png/250px-Yas_Marina_Circuit.png</v>
       </c>
       <c r="I77" t="str">
-        <f>VLOOKUP(B77,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://www.racefans.net/wp-content/uploads/2021/07/racefansdotnet-21-07-24-21-06-40-1.jpg</v>
+        <f>VLOOKUP(B77,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e1/Yas_Marina_Circuit%2C_October_12%2C_2018_SkySat_%28cropped%29.jpg/220px-Yas_Marina_Circuit%2C_October_12%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -3544,12 +3544,12 @@
         <v>100</v>
       </c>
       <c r="H78" t="str">
-        <f>VLOOKUP(B78,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/4c/Losail.svg/250px-Losail.svg.png</v>
+        <f>VLOOKUP(B78,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/2/29/Korea_international_circuit_v3.svg/260px-Korea_international_circuit_v3.svg.png</v>
       </c>
       <c r="I78" t="str">
-        <f>VLOOKUP(B78,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://www.racefans.net/wp-content/uploads/2021/07/racefansdotnet-21-07-24-21-06-40-1.jpg</v>
+        <f>VLOOKUP(B78,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcSb2epC9a8qoZyccNJCgRnRtPYPEDOhbu7C3A&amp;usqp=CAU</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -3575,11 +3575,11 @@
         <v>11</v>
       </c>
       <c r="H79" t="str">
-        <f>VLOOKUP(B79,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B79,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0a/Albert_Park_Circuit_2021.svg/220px-Albert_Park_Circuit_2021.svg.png</v>
       </c>
       <c r="I79" t="str">
-        <f>VLOOKUP(B79,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B79,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8e/Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -3606,12 +3606,12 @@
         <v>114</v>
       </c>
       <c r="H80" t="str">
-        <f>VLOOKUP(B80,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0a/Albert_Park_Circuit_2021.svg/220px-Albert_Park_Circuit_2021.svg.png</v>
+        <f>VLOOKUP(B80,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/a/a5/Austin_circuit.svg/250px-Austin_circuit.svg.png</v>
       </c>
       <c r="I80" t="str">
-        <f>VLOOKUP(B80,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8e/Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B80,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/78/Circuit_of_the_Americas%2C_April_22%2C_2018_SkySat_%28cropped2%29.jpg/220px-Circuit_of_the_Americas%2C_April_22%2C_2018_SkySat_%28cropped2%29.jpg</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -3637,11 +3637,11 @@
         <v>16</v>
       </c>
       <c r="H81" t="str">
-        <f>VLOOKUP(B81,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B81,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/en/thumb/d/d1/Bahrain_International_Circuit_logo.png/200px-Bahrain_International_Circuit_logo.png</v>
       </c>
       <c r="I81" t="str">
-        <f>VLOOKUP(B81,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B81,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bc/Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg/220px-Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -3668,11 +3668,11 @@
         <v>21</v>
       </c>
       <c r="H82" t="str">
-        <f>VLOOKUP(B82,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B82,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/87/Circuit_de_Catalunya_moto_2021.svg/250px-Circuit_de_Catalunya_moto_2021.svg.png</v>
       </c>
       <c r="I82" t="str">
-        <f>VLOOKUP(B82,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B82,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e7/Circuit_de_Barcelona-Catalunya%2C_April_19%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Barcelona-Catalunya%2C_April_19%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -3699,11 +3699,11 @@
         <v>26</v>
       </c>
       <c r="H83" t="str">
-        <f>VLOOKUP(B83,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B83,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e5/Hockenheim2012.svg/220px-Hockenheim2012.svg.png</v>
       </c>
       <c r="I83" t="str">
-        <f>VLOOKUP(B83,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B83,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/41/Hockenheimring%2C_April_29%2C_2018_SkySat_%28crop%29.jpg/220px-Hockenheimring%2C_April_29%2C_2018_SkySat_%28crop%29.jpg</v>
       </c>
     </row>
@@ -3730,11 +3730,11 @@
         <v>31</v>
       </c>
       <c r="H84" t="str">
-        <f>VLOOKUP(B84,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B84,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/91/Hungaroring.svg/260px-Hungaroring.svg.png</v>
       </c>
       <c r="I84" t="str">
-        <f>VLOOKUP(B84,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B84,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/a/aa/Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg/220px-Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -3761,11 +3761,11 @@
         <v>36</v>
       </c>
       <c r="H85" t="str">
-        <f>VLOOKUP(B85,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B85,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/cf/Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace_%28AKA_Interlagos%29_track_map.svg/260px-Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace_%28AKA_Interlagos%29_track_map.svg.png</v>
       </c>
       <c r="I85" t="str">
-        <f>VLOOKUP(B85,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B85,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/70/Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace%2C_July_3%2C_2018_SkySat_%28cropped%29.jpg/220px-Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace%2C_July_3%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -3792,11 +3792,11 @@
         <v>46</v>
       </c>
       <c r="H86" t="str">
-        <f>VLOOKUP(B86,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B86,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/17/Planned_2023_Marina_Bay_Street_Circuit_layout.png/220px-Planned_2023_Marina_Bay_Street_Circuit_layout.png</v>
       </c>
       <c r="I86" t="str">
-        <f>VLOOKUP(B86,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B86,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f0/1_singapore_f1_night_race_2012_city_skyline.jpg/240px-1_singapore_f1_night_race_2012_city_skyline.jpg</v>
       </c>
     </row>
@@ -3823,11 +3823,11 @@
         <v>51</v>
       </c>
       <c r="H87" t="str">
-        <f>VLOOKUP(B87,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B87,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/3/36/Monte_Carlo_Formula_1_track_map.svg/250px-Monte_Carlo_Formula_1_track_map.svg.png</v>
       </c>
       <c r="I87" t="str">
-        <f>VLOOKUP(B87,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B87,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/c7/Circuit_de_Monaco%2C_April_1%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Monaco%2C_April_1%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -3854,11 +3854,11 @@
         <v>56</v>
       </c>
       <c r="H88" t="str">
-        <f>VLOOKUP(B88,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B88,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
       </c>
       <c r="I88" t="str">
-        <f>VLOOKUP(B88,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B88,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -3885,12 +3885,12 @@
         <v>119</v>
       </c>
       <c r="H89" t="str">
-        <f>VLOOKUP(B89,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
+        <f>VLOOKUP(B89,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/9c/%C3%96sterreichring-A1Ring.svg/400px-%C3%96sterreichring-A1Ring.svg.png</v>
       </c>
       <c r="I89" t="str">
-        <f>VLOOKUP(B89,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B89,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/cb/Luftaufnahme_%28c%29Red_Bull_Ring.jpg/600px-Luftaufnahme_%28c%29Red_Bull_Ring.jpg</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -3916,11 +3916,11 @@
         <v>61</v>
       </c>
       <c r="H90" t="str">
-        <f>VLOOKUP(B90,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B90,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/67/Sepang.svg/250px-Sepang.svg.png</v>
       </c>
       <c r="I90" t="str">
-        <f>VLOOKUP(B90,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B90,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/7f/Sepang_International_Circuit_1.JPG/220px-Sepang_International_Circuit_1.JPG</v>
       </c>
     </row>
@@ -3947,11 +3947,11 @@
         <v>66</v>
       </c>
       <c r="H91" t="str">
-        <f>VLOOKUP(B91,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B91,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/14/Shanghai_International_Racing_Circuit_track_map.svg/250px-Shanghai_International_Racing_Circuit_track_map.svg.png</v>
       </c>
       <c r="I91" t="str">
-        <f>VLOOKUP(B91,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B91,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/d/d6/Shanghai_International_Circuit%2C_April_7%2C_2018_SkySat_%28rotated%29.jpg/220px-Shanghai_International_Circuit%2C_April_7%2C_2018_SkySat_%28rotated%29.jpg</v>
       </c>
     </row>
@@ -3978,11 +3978,11 @@
         <v>71</v>
       </c>
       <c r="H92" t="str">
-        <f>VLOOKUP(B92,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B92,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bd/Silverstone_Circuit_2020.png/250px-Silverstone_Circuit_2020.png</v>
       </c>
       <c r="I92" t="str">
-        <f>VLOOKUP(B92,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B92,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8d/Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg/220px-Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -4009,12 +4009,12 @@
         <v>124</v>
       </c>
       <c r="H93" t="str">
-        <f>VLOOKUP(B93,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bd/Silverstone_Circuit_2020.png/250px-Silverstone_Circuit_2020.png</v>
+        <f>VLOOKUP(B93,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/d/d3/Circuit_Sochi.svg/250px-Circuit_Sochi.svg.png</v>
       </c>
       <c r="I93" t="str">
-        <f>VLOOKUP(B93,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8d/Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg/220px-Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B93,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/16/Sochi_Autodrom%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg/220px-Sochi_Autodrom%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -4040,11 +4040,11 @@
         <v>76</v>
       </c>
       <c r="H94" t="str">
-        <f>VLOOKUP(B94,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B94,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/5/54/Spa-Francorchamps_of_Belgium.svg/260px-Spa-Francorchamps_of_Belgium.svg.png</v>
       </c>
       <c r="I94" t="str">
-        <f>VLOOKUP(B94,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B94,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/77/Circuit_de_Spa-Francorchamps%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Spa-Francorchamps%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -4071,11 +4071,11 @@
         <v>81</v>
       </c>
       <c r="H95" t="str">
-        <f>VLOOKUP(B95,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B95,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/ec/Suzuka_circuit_map--2005.svg/260px-Suzuka_circuit_map--2005.svg.png</v>
       </c>
       <c r="I95" t="str">
-        <f>VLOOKUP(B95,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B95,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/9a/Suzuka_International_Racing_Course%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg/220px-Suzuka_International_Racing_Course%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -4102,11 +4102,11 @@
         <v>90</v>
       </c>
       <c r="H96" t="str">
-        <f>VLOOKUP(B96,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B96,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f9/%C3%8Ele_Notre-Dame_%28Circuit_Gilles_Villeneuve%29.svg/280px-%C3%8Ele_Notre-Dame_%28Circuit_Gilles_Villeneuve%29.svg.png</v>
       </c>
       <c r="I96" t="str">
-        <f>VLOOKUP(B96,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B96,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/3/38/F1_1978_circuit_ile_notre_dame.png/220px-F1_1978_circuit_ile_notre_dame.png</v>
       </c>
     </row>
@@ -4133,12 +4133,12 @@
         <v>95</v>
       </c>
       <c r="H97" t="str">
-        <f>VLOOKUP(B97,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/4c/Losail.svg/250px-Losail.svg.png</v>
+        <f>VLOOKUP(B97,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/b0/Yas_Marina_Circuit.png/250px-Yas_Marina_Circuit.png</v>
       </c>
       <c r="I97" t="str">
-        <f>VLOOKUP(B97,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://www.racefans.net/wp-content/uploads/2021/07/racefansdotnet-21-07-24-21-06-40-1.jpg</v>
+        <f>VLOOKUP(B97,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e1/Yas_Marina_Circuit%2C_October_12%2C_2018_SkySat_%28cropped%29.jpg/220px-Yas_Marina_Circuit%2C_October_12%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -4164,11 +4164,11 @@
         <v>11</v>
       </c>
       <c r="H98" t="str">
-        <f>VLOOKUP(B98,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B98,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0a/Albert_Park_Circuit_2021.svg/220px-Albert_Park_Circuit_2021.svg.png</v>
       </c>
       <c r="I98" t="str">
-        <f>VLOOKUP(B98,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B98,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8e/Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -4195,12 +4195,12 @@
         <v>114</v>
       </c>
       <c r="H99" t="str">
-        <f>VLOOKUP(B99,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0a/Albert_Park_Circuit_2021.svg/220px-Albert_Park_Circuit_2021.svg.png</v>
+        <f>VLOOKUP(B99,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/a/a5/Austin_circuit.svg/250px-Austin_circuit.svg.png</v>
       </c>
       <c r="I99" t="str">
-        <f>VLOOKUP(B99,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8e/Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B99,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/78/Circuit_of_the_Americas%2C_April_22%2C_2018_SkySat_%28cropped2%29.jpg/220px-Circuit_of_the_Americas%2C_April_22%2C_2018_SkySat_%28cropped2%29.jpg</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -4226,11 +4226,11 @@
         <v>16</v>
       </c>
       <c r="H100" t="str">
-        <f>VLOOKUP(B100,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B100,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/en/thumb/d/d1/Bahrain_International_Circuit_logo.png/200px-Bahrain_International_Circuit_logo.png</v>
       </c>
       <c r="I100" t="str">
-        <f>VLOOKUP(B100,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B100,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bc/Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg/220px-Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -4257,11 +4257,11 @@
         <v>21</v>
       </c>
       <c r="H101" t="str">
-        <f>VLOOKUP(B101,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B101,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/87/Circuit_de_Catalunya_moto_2021.svg/250px-Circuit_de_Catalunya_moto_2021.svg.png</v>
       </c>
       <c r="I101" t="str">
-        <f>VLOOKUP(B101,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B101,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e7/Circuit_de_Barcelona-Catalunya%2C_April_19%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Barcelona-Catalunya%2C_April_19%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -4288,11 +4288,11 @@
         <v>31</v>
       </c>
       <c r="H102" t="str">
-        <f>VLOOKUP(B102,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B102,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/91/Hungaroring.svg/260px-Hungaroring.svg.png</v>
       </c>
       <c r="I102" t="str">
-        <f>VLOOKUP(B102,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B102,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/a/aa/Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg/220px-Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -4319,11 +4319,11 @@
         <v>36</v>
       </c>
       <c r="H103" t="str">
-        <f>VLOOKUP(B103,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B103,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/cf/Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace_%28AKA_Interlagos%29_track_map.svg/260px-Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace_%28AKA_Interlagos%29_track_map.svg.png</v>
       </c>
       <c r="I103" t="str">
-        <f>VLOOKUP(B103,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B103,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/70/Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace%2C_July_3%2C_2018_SkySat_%28cropped%29.jpg/220px-Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace%2C_July_3%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -4350,11 +4350,11 @@
         <v>46</v>
       </c>
       <c r="H104" t="str">
-        <f>VLOOKUP(B104,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B104,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/17/Planned_2023_Marina_Bay_Street_Circuit_layout.png/220px-Planned_2023_Marina_Bay_Street_Circuit_layout.png</v>
       </c>
       <c r="I104" t="str">
-        <f>VLOOKUP(B104,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B104,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f0/1_singapore_f1_night_race_2012_city_skyline.jpg/240px-1_singapore_f1_night_race_2012_city_skyline.jpg</v>
       </c>
     </row>
@@ -4381,11 +4381,11 @@
         <v>51</v>
       </c>
       <c r="H105" t="str">
-        <f>VLOOKUP(B105,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B105,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/3/36/Monte_Carlo_Formula_1_track_map.svg/250px-Monte_Carlo_Formula_1_track_map.svg.png</v>
       </c>
       <c r="I105" t="str">
-        <f>VLOOKUP(B105,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B105,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/c7/Circuit_de_Monaco%2C_April_1%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Monaco%2C_April_1%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -4412,11 +4412,11 @@
         <v>56</v>
       </c>
       <c r="H106" t="str">
-        <f>VLOOKUP(B106,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B106,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
       </c>
       <c r="I106" t="str">
-        <f>VLOOKUP(B106,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B106,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -4443,12 +4443,12 @@
         <v>119</v>
       </c>
       <c r="H107" t="str">
-        <f>VLOOKUP(B107,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
+        <f>VLOOKUP(B107,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/9c/%C3%96sterreichring-A1Ring.svg/400px-%C3%96sterreichring-A1Ring.svg.png</v>
       </c>
       <c r="I107" t="str">
-        <f>VLOOKUP(B107,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B107,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/cb/Luftaufnahme_%28c%29Red_Bull_Ring.jpg/600px-Luftaufnahme_%28c%29Red_Bull_Ring.jpg</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -4474,12 +4474,12 @@
         <v>129</v>
       </c>
       <c r="H108" t="str">
-        <f>VLOOKUP(B108,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
+        <f>VLOOKUP(B108,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/c6/Autodromo_Hermanos_Rodriguez_%28Formula_E_Layout_2023%29.png/250px-Autodromo_Hermanos_Rodriguez_%28Formula_E_Layout_2023%29.png</v>
       </c>
       <c r="I108" t="str">
-        <f>VLOOKUP(B108,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B108,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f6/Aut%C3%B3dromo_Hermanos_Rodr%C3%ADguez%2C_June_4%2C_2018_SkySat_%28cropped%29.jpg/220px-Aut%C3%B3dromo_Hermanos_Rodr%C3%ADguez%2C_June_4%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
@@ -4505,11 +4505,11 @@
         <v>61</v>
       </c>
       <c r="H109" t="str">
-        <f>VLOOKUP(B109,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B109,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/67/Sepang.svg/250px-Sepang.svg.png</v>
       </c>
       <c r="I109" t="str">
-        <f>VLOOKUP(B109,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B109,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/7f/Sepang_International_Circuit_1.JPG/220px-Sepang_International_Circuit_1.JPG</v>
       </c>
     </row>
@@ -4536,11 +4536,11 @@
         <v>66</v>
       </c>
       <c r="H110" t="str">
-        <f>VLOOKUP(B110,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B110,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/14/Shanghai_International_Racing_Circuit_track_map.svg/250px-Shanghai_International_Racing_Circuit_track_map.svg.png</v>
       </c>
       <c r="I110" t="str">
-        <f>VLOOKUP(B110,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B110,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/d/d6/Shanghai_International_Circuit%2C_April_7%2C_2018_SkySat_%28rotated%29.jpg/220px-Shanghai_International_Circuit%2C_April_7%2C_2018_SkySat_%28rotated%29.jpg</v>
       </c>
     </row>
@@ -4567,11 +4567,11 @@
         <v>71</v>
       </c>
       <c r="H111" t="str">
-        <f>VLOOKUP(B111,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B111,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bd/Silverstone_Circuit_2020.png/250px-Silverstone_Circuit_2020.png</v>
       </c>
       <c r="I111" t="str">
-        <f>VLOOKUP(B111,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B111,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8d/Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg/220px-Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -4598,12 +4598,12 @@
         <v>124</v>
       </c>
       <c r="H112" t="str">
-        <f>VLOOKUP(B112,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bd/Silverstone_Circuit_2020.png/250px-Silverstone_Circuit_2020.png</v>
+        <f>VLOOKUP(B112,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/d/d3/Circuit_Sochi.svg/250px-Circuit_Sochi.svg.png</v>
       </c>
       <c r="I112" t="str">
-        <f>VLOOKUP(B112,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8d/Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg/220px-Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B112,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/16/Sochi_Autodrom%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg/220px-Sochi_Autodrom%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
@@ -4629,11 +4629,11 @@
         <v>76</v>
       </c>
       <c r="H113" t="str">
-        <f>VLOOKUP(B113,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B113,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/5/54/Spa-Francorchamps_of_Belgium.svg/260px-Spa-Francorchamps_of_Belgium.svg.png</v>
       </c>
       <c r="I113" t="str">
-        <f>VLOOKUP(B113,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B113,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/77/Circuit_de_Spa-Francorchamps%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Spa-Francorchamps%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -4660,11 +4660,11 @@
         <v>81</v>
       </c>
       <c r="H114" t="str">
-        <f>VLOOKUP(B114,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B114,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/ec/Suzuka_circuit_map--2005.svg/260px-Suzuka_circuit_map--2005.svg.png</v>
       </c>
       <c r="I114" t="str">
-        <f>VLOOKUP(B114,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B114,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/9a/Suzuka_International_Racing_Course%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg/220px-Suzuka_International_Racing_Course%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -4691,11 +4691,11 @@
         <v>90</v>
       </c>
       <c r="H115" t="str">
-        <f>VLOOKUP(B115,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B115,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f9/%C3%8Ele_Notre-Dame_%28Circuit_Gilles_Villeneuve%29.svg/280px-%C3%8Ele_Notre-Dame_%28Circuit_Gilles_Villeneuve%29.svg.png</v>
       </c>
       <c r="I115" t="str">
-        <f>VLOOKUP(B115,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B115,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/3/38/F1_1978_circuit_ile_notre_dame.png/220px-F1_1978_circuit_ile_notre_dame.png</v>
       </c>
     </row>
@@ -4722,12 +4722,12 @@
         <v>95</v>
       </c>
       <c r="H116" t="str">
-        <f>VLOOKUP(B116,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/4c/Losail.svg/250px-Losail.svg.png</v>
+        <f>VLOOKUP(B116,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/b0/Yas_Marina_Circuit.png/250px-Yas_Marina_Circuit.png</v>
       </c>
       <c r="I116" t="str">
-        <f>VLOOKUP(B116,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://www.racefans.net/wp-content/uploads/2021/07/racefansdotnet-21-07-24-21-06-40-1.jpg</v>
+        <f>VLOOKUP(B116,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e1/Yas_Marina_Circuit%2C_October_12%2C_2018_SkySat_%28cropped%29.jpg/220px-Yas_Marina_Circuit%2C_October_12%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -4753,11 +4753,11 @@
         <v>11</v>
       </c>
       <c r="H117" t="str">
-        <f>VLOOKUP(B117,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B117,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0a/Albert_Park_Circuit_2021.svg/220px-Albert_Park_Circuit_2021.svg.png</v>
       </c>
       <c r="I117" t="str">
-        <f>VLOOKUP(B117,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B117,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8e/Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -4784,12 +4784,12 @@
         <v>114</v>
       </c>
       <c r="H118" t="str">
-        <f>VLOOKUP(B118,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0a/Albert_Park_Circuit_2021.svg/220px-Albert_Park_Circuit_2021.svg.png</v>
+        <f>VLOOKUP(B118,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/a/a5/Austin_circuit.svg/250px-Austin_circuit.svg.png</v>
       </c>
       <c r="I118" t="str">
-        <f>VLOOKUP(B118,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8e/Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B118,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/78/Circuit_of_the_Americas%2C_April_22%2C_2018_SkySat_%28cropped2%29.jpg/220px-Circuit_of_the_Americas%2C_April_22%2C_2018_SkySat_%28cropped2%29.jpg</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -4815,11 +4815,11 @@
         <v>16</v>
       </c>
       <c r="H119" t="str">
-        <f>VLOOKUP(B119,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B119,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/en/thumb/d/d1/Bahrain_International_Circuit_logo.png/200px-Bahrain_International_Circuit_logo.png</v>
       </c>
       <c r="I119" t="str">
-        <f>VLOOKUP(B119,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B119,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bc/Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg/220px-Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -4846,12 +4846,12 @@
         <v>134</v>
       </c>
       <c r="H120" t="str">
-        <f>VLOOKUP(B120,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/en/thumb/d/d1/Bahrain_International_Circuit_logo.png/200px-Bahrain_International_Circuit_logo.png</v>
+        <f>VLOOKUP(B120,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f1/Baku_Formula_One_circuit_map.svg/300px-Baku_Formula_One_circuit_map.svg.png</v>
       </c>
       <c r="I120" t="str">
-        <f>VLOOKUP(B120,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bc/Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg/220px-Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B120,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/76/Baku-F1-Street-Circuit-Openstreetmaps-rev1.png/220px-Baku-F1-Street-Circuit-Openstreetmaps-rev1.png</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -4877,11 +4877,11 @@
         <v>21</v>
       </c>
       <c r="H121" t="str">
-        <f>VLOOKUP(B121,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B121,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/87/Circuit_de_Catalunya_moto_2021.svg/250px-Circuit_de_Catalunya_moto_2021.svg.png</v>
       </c>
       <c r="I121" t="str">
-        <f>VLOOKUP(B121,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B121,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e7/Circuit_de_Barcelona-Catalunya%2C_April_19%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Barcelona-Catalunya%2C_April_19%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -4908,11 +4908,11 @@
         <v>26</v>
       </c>
       <c r="H122" t="str">
-        <f>VLOOKUP(B122,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B122,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e5/Hockenheim2012.svg/220px-Hockenheim2012.svg.png</v>
       </c>
       <c r="I122" t="str">
-        <f>VLOOKUP(B122,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B122,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/41/Hockenheimring%2C_April_29%2C_2018_SkySat_%28crop%29.jpg/220px-Hockenheimring%2C_April_29%2C_2018_SkySat_%28crop%29.jpg</v>
       </c>
     </row>
@@ -4939,11 +4939,11 @@
         <v>31</v>
       </c>
       <c r="H123" t="str">
-        <f>VLOOKUP(B123,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B123,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/91/Hungaroring.svg/260px-Hungaroring.svg.png</v>
       </c>
       <c r="I123" t="str">
-        <f>VLOOKUP(B123,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B123,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/a/aa/Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg/220px-Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -4970,11 +4970,11 @@
         <v>36</v>
       </c>
       <c r="H124" t="str">
-        <f>VLOOKUP(B124,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B124,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/cf/Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace_%28AKA_Interlagos%29_track_map.svg/260px-Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace_%28AKA_Interlagos%29_track_map.svg.png</v>
       </c>
       <c r="I124" t="str">
-        <f>VLOOKUP(B124,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B124,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/70/Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace%2C_July_3%2C_2018_SkySat_%28cropped%29.jpg/220px-Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace%2C_July_3%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -5001,11 +5001,11 @@
         <v>46</v>
       </c>
       <c r="H125" t="str">
-        <f>VLOOKUP(B125,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B125,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/17/Planned_2023_Marina_Bay_Street_Circuit_layout.png/220px-Planned_2023_Marina_Bay_Street_Circuit_layout.png</v>
       </c>
       <c r="I125" t="str">
-        <f>VLOOKUP(B125,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B125,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f0/1_singapore_f1_night_race_2012_city_skyline.jpg/240px-1_singapore_f1_night_race_2012_city_skyline.jpg</v>
       </c>
     </row>
@@ -5032,11 +5032,11 @@
         <v>51</v>
       </c>
       <c r="H126" t="str">
-        <f>VLOOKUP(B126,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B126,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/3/36/Monte_Carlo_Formula_1_track_map.svg/250px-Monte_Carlo_Formula_1_track_map.svg.png</v>
       </c>
       <c r="I126" t="str">
-        <f>VLOOKUP(B126,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B126,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/c7/Circuit_de_Monaco%2C_April_1%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Monaco%2C_April_1%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -5063,11 +5063,11 @@
         <v>56</v>
       </c>
       <c r="H127" t="str">
-        <f>VLOOKUP(B127,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B127,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
       </c>
       <c r="I127" t="str">
-        <f>VLOOKUP(B127,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B127,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -5094,12 +5094,12 @@
         <v>119</v>
       </c>
       <c r="H128" t="str">
-        <f>VLOOKUP(B128,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
+        <f>VLOOKUP(B128,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/9c/%C3%96sterreichring-A1Ring.svg/400px-%C3%96sterreichring-A1Ring.svg.png</v>
       </c>
       <c r="I128" t="str">
-        <f>VLOOKUP(B128,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B128,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/cb/Luftaufnahme_%28c%29Red_Bull_Ring.jpg/600px-Luftaufnahme_%28c%29Red_Bull_Ring.jpg</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -5125,12 +5125,12 @@
         <v>129</v>
       </c>
       <c r="H129" t="str">
-        <f>VLOOKUP(B129,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
+        <f>VLOOKUP(B129,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/c6/Autodromo_Hermanos_Rodriguez_%28Formula_E_Layout_2023%29.png/250px-Autodromo_Hermanos_Rodriguez_%28Formula_E_Layout_2023%29.png</v>
       </c>
       <c r="I129" t="str">
-        <f>VLOOKUP(B129,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B129,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f6/Aut%C3%B3dromo_Hermanos_Rodr%C3%ADguez%2C_June_4%2C_2018_SkySat_%28cropped%29.jpg/220px-Aut%C3%B3dromo_Hermanos_Rodr%C3%ADguez%2C_June_4%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -5156,11 +5156,11 @@
         <v>61</v>
       </c>
       <c r="H130" t="str">
-        <f>VLOOKUP(B130,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B130,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/67/Sepang.svg/250px-Sepang.svg.png</v>
       </c>
       <c r="I130" t="str">
-        <f>VLOOKUP(B130,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B130,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/7f/Sepang_International_Circuit_1.JPG/220px-Sepang_International_Circuit_1.JPG</v>
       </c>
     </row>
@@ -5187,11 +5187,11 @@
         <v>66</v>
       </c>
       <c r="H131" t="str">
-        <f>VLOOKUP(B131,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B131,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/14/Shanghai_International_Racing_Circuit_track_map.svg/250px-Shanghai_International_Racing_Circuit_track_map.svg.png</v>
       </c>
       <c r="I131" t="str">
-        <f>VLOOKUP(B131,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B131,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/d/d6/Shanghai_International_Circuit%2C_April_7%2C_2018_SkySat_%28rotated%29.jpg/220px-Shanghai_International_Circuit%2C_April_7%2C_2018_SkySat_%28rotated%29.jpg</v>
       </c>
     </row>
@@ -5218,11 +5218,11 @@
         <v>71</v>
       </c>
       <c r="H132" t="str">
-        <f>VLOOKUP(B132,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B132,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bd/Silverstone_Circuit_2020.png/250px-Silverstone_Circuit_2020.png</v>
       </c>
       <c r="I132" t="str">
-        <f>VLOOKUP(B132,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B132,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8d/Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg/220px-Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -5249,12 +5249,12 @@
         <v>124</v>
       </c>
       <c r="H133" t="str">
-        <f>VLOOKUP(B133,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bd/Silverstone_Circuit_2020.png/250px-Silverstone_Circuit_2020.png</v>
+        <f>VLOOKUP(B133,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/d/d3/Circuit_Sochi.svg/250px-Circuit_Sochi.svg.png</v>
       </c>
       <c r="I133" t="str">
-        <f>VLOOKUP(B133,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8d/Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg/220px-Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B133,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/16/Sochi_Autodrom%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg/220px-Sochi_Autodrom%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
@@ -5280,11 +5280,11 @@
         <v>76</v>
       </c>
       <c r="H134" t="str">
-        <f>VLOOKUP(B134,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B134,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/5/54/Spa-Francorchamps_of_Belgium.svg/260px-Spa-Francorchamps_of_Belgium.svg.png</v>
       </c>
       <c r="I134" t="str">
-        <f>VLOOKUP(B134,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B134,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/77/Circuit_de_Spa-Francorchamps%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Spa-Francorchamps%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -5311,11 +5311,11 @@
         <v>81</v>
       </c>
       <c r="H135" t="str">
-        <f>VLOOKUP(B135,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B135,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/ec/Suzuka_circuit_map--2005.svg/260px-Suzuka_circuit_map--2005.svg.png</v>
       </c>
       <c r="I135" t="str">
-        <f>VLOOKUP(B135,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B135,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/9a/Suzuka_International_Racing_Course%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg/220px-Suzuka_International_Racing_Course%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -5342,11 +5342,11 @@
         <v>90</v>
       </c>
       <c r="H136" t="str">
-        <f>VLOOKUP(B136,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B136,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f9/%C3%8Ele_Notre-Dame_%28Circuit_Gilles_Villeneuve%29.svg/280px-%C3%8Ele_Notre-Dame_%28Circuit_Gilles_Villeneuve%29.svg.png</v>
       </c>
       <c r="I136" t="str">
-        <f>VLOOKUP(B136,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B136,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/3/38/F1_1978_circuit_ile_notre_dame.png/220px-F1_1978_circuit_ile_notre_dame.png</v>
       </c>
     </row>
@@ -5373,12 +5373,12 @@
         <v>95</v>
       </c>
       <c r="H137" t="str">
-        <f>VLOOKUP(B137,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/4c/Losail.svg/250px-Losail.svg.png</v>
+        <f>VLOOKUP(B137,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/b0/Yas_Marina_Circuit.png/250px-Yas_Marina_Circuit.png</v>
       </c>
       <c r="I137" t="str">
-        <f>VLOOKUP(B137,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://www.racefans.net/wp-content/uploads/2021/07/racefansdotnet-21-07-24-21-06-40-1.jpg</v>
+        <f>VLOOKUP(B137,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e1/Yas_Marina_Circuit%2C_October_12%2C_2018_SkySat_%28cropped%29.jpg/220px-Yas_Marina_Circuit%2C_October_12%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
@@ -5404,11 +5404,11 @@
         <v>11</v>
       </c>
       <c r="H138" t="str">
-        <f>VLOOKUP(B138,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B138,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0a/Albert_Park_Circuit_2021.svg/220px-Albert_Park_Circuit_2021.svg.png</v>
       </c>
       <c r="I138" t="str">
-        <f>VLOOKUP(B138,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B138,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8e/Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -5435,12 +5435,12 @@
         <v>114</v>
       </c>
       <c r="H139" t="str">
-        <f>VLOOKUP(B139,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0a/Albert_Park_Circuit_2021.svg/220px-Albert_Park_Circuit_2021.svg.png</v>
+        <f>VLOOKUP(B139,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/a/a5/Austin_circuit.svg/250px-Austin_circuit.svg.png</v>
       </c>
       <c r="I139" t="str">
-        <f>VLOOKUP(B139,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8e/Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B139,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/78/Circuit_of_the_Americas%2C_April_22%2C_2018_SkySat_%28cropped2%29.jpg/220px-Circuit_of_the_Americas%2C_April_22%2C_2018_SkySat_%28cropped2%29.jpg</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
@@ -5466,11 +5466,11 @@
         <v>16</v>
       </c>
       <c r="H140" t="str">
-        <f>VLOOKUP(B140,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B140,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/en/thumb/d/d1/Bahrain_International_Circuit_logo.png/200px-Bahrain_International_Circuit_logo.png</v>
       </c>
       <c r="I140" t="str">
-        <f>VLOOKUP(B140,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B140,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bc/Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg/220px-Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -5497,12 +5497,12 @@
         <v>134</v>
       </c>
       <c r="H141" t="str">
-        <f>VLOOKUP(B141,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/en/thumb/d/d1/Bahrain_International_Circuit_logo.png/200px-Bahrain_International_Circuit_logo.png</v>
+        <f>VLOOKUP(B141,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f1/Baku_Formula_One_circuit_map.svg/300px-Baku_Formula_One_circuit_map.svg.png</v>
       </c>
       <c r="I141" t="str">
-        <f>VLOOKUP(B141,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bc/Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg/220px-Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B141,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/76/Baku-F1-Street-Circuit-Openstreetmaps-rev1.png/220px-Baku-F1-Street-Circuit-Openstreetmaps-rev1.png</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
@@ -5528,11 +5528,11 @@
         <v>21</v>
       </c>
       <c r="H142" t="str">
-        <f>VLOOKUP(B142,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B142,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/87/Circuit_de_Catalunya_moto_2021.svg/250px-Circuit_de_Catalunya_moto_2021.svg.png</v>
       </c>
       <c r="I142" t="str">
-        <f>VLOOKUP(B142,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B142,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e7/Circuit_de_Barcelona-Catalunya%2C_April_19%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Barcelona-Catalunya%2C_April_19%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -5559,11 +5559,11 @@
         <v>31</v>
       </c>
       <c r="H143" t="str">
-        <f>VLOOKUP(B143,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B143,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/91/Hungaroring.svg/260px-Hungaroring.svg.png</v>
       </c>
       <c r="I143" t="str">
-        <f>VLOOKUP(B143,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B143,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/a/aa/Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg/220px-Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -5590,11 +5590,11 @@
         <v>36</v>
       </c>
       <c r="H144" t="str">
-        <f>VLOOKUP(B144,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B144,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/cf/Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace_%28AKA_Interlagos%29_track_map.svg/260px-Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace_%28AKA_Interlagos%29_track_map.svg.png</v>
       </c>
       <c r="I144" t="str">
-        <f>VLOOKUP(B144,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B144,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/70/Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace%2C_July_3%2C_2018_SkySat_%28cropped%29.jpg/220px-Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace%2C_July_3%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -5621,11 +5621,11 @@
         <v>46</v>
       </c>
       <c r="H145" t="str">
-        <f>VLOOKUP(B145,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B145,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/17/Planned_2023_Marina_Bay_Street_Circuit_layout.png/220px-Planned_2023_Marina_Bay_Street_Circuit_layout.png</v>
       </c>
       <c r="I145" t="str">
-        <f>VLOOKUP(B145,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B145,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f0/1_singapore_f1_night_race_2012_city_skyline.jpg/240px-1_singapore_f1_night_race_2012_city_skyline.jpg</v>
       </c>
     </row>
@@ -5652,11 +5652,11 @@
         <v>51</v>
       </c>
       <c r="H146" t="str">
-        <f>VLOOKUP(B146,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B146,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/3/36/Monte_Carlo_Formula_1_track_map.svg/250px-Monte_Carlo_Formula_1_track_map.svg.png</v>
       </c>
       <c r="I146" t="str">
-        <f>VLOOKUP(B146,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B146,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/c7/Circuit_de_Monaco%2C_April_1%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Monaco%2C_April_1%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -5683,11 +5683,11 @@
         <v>56</v>
       </c>
       <c r="H147" t="str">
-        <f>VLOOKUP(B147,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B147,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
       </c>
       <c r="I147" t="str">
-        <f>VLOOKUP(B147,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B147,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -5714,12 +5714,12 @@
         <v>119</v>
       </c>
       <c r="H148" t="str">
-        <f>VLOOKUP(B148,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
+        <f>VLOOKUP(B148,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/9c/%C3%96sterreichring-A1Ring.svg/400px-%C3%96sterreichring-A1Ring.svg.png</v>
       </c>
       <c r="I148" t="str">
-        <f>VLOOKUP(B148,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B148,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/cb/Luftaufnahme_%28c%29Red_Bull_Ring.jpg/600px-Luftaufnahme_%28c%29Red_Bull_Ring.jpg</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
@@ -5745,12 +5745,12 @@
         <v>129</v>
       </c>
       <c r="H149" t="str">
-        <f>VLOOKUP(B149,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
+        <f>VLOOKUP(B149,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/c6/Autodromo_Hermanos_Rodriguez_%28Formula_E_Layout_2023%29.png/250px-Autodromo_Hermanos_Rodriguez_%28Formula_E_Layout_2023%29.png</v>
       </c>
       <c r="I149" t="str">
-        <f>VLOOKUP(B149,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B149,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f6/Aut%C3%B3dromo_Hermanos_Rodr%C3%ADguez%2C_June_4%2C_2018_SkySat_%28cropped%29.jpg/220px-Aut%C3%B3dromo_Hermanos_Rodr%C3%ADguez%2C_June_4%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
@@ -5776,11 +5776,11 @@
         <v>61</v>
       </c>
       <c r="H150" t="str">
-        <f>VLOOKUP(B150,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B150,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/67/Sepang.svg/250px-Sepang.svg.png</v>
       </c>
       <c r="I150" t="str">
-        <f>VLOOKUP(B150,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B150,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/7f/Sepang_International_Circuit_1.JPG/220px-Sepang_International_Circuit_1.JPG</v>
       </c>
     </row>
@@ -5807,11 +5807,11 @@
         <v>66</v>
       </c>
       <c r="H151" t="str">
-        <f>VLOOKUP(B151,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B151,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/14/Shanghai_International_Racing_Circuit_track_map.svg/250px-Shanghai_International_Racing_Circuit_track_map.svg.png</v>
       </c>
       <c r="I151" t="str">
-        <f>VLOOKUP(B151,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B151,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/d/d6/Shanghai_International_Circuit%2C_April_7%2C_2018_SkySat_%28rotated%29.jpg/220px-Shanghai_International_Circuit%2C_April_7%2C_2018_SkySat_%28rotated%29.jpg</v>
       </c>
     </row>
@@ -5838,11 +5838,11 @@
         <v>71</v>
       </c>
       <c r="H152" t="str">
-        <f>VLOOKUP(B152,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B152,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bd/Silverstone_Circuit_2020.png/250px-Silverstone_Circuit_2020.png</v>
       </c>
       <c r="I152" t="str">
-        <f>VLOOKUP(B152,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B152,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8d/Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg/220px-Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -5869,12 +5869,12 @@
         <v>124</v>
       </c>
       <c r="H153" t="str">
-        <f>VLOOKUP(B153,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bd/Silverstone_Circuit_2020.png/250px-Silverstone_Circuit_2020.png</v>
+        <f>VLOOKUP(B153,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/d/d3/Circuit_Sochi.svg/250px-Circuit_Sochi.svg.png</v>
       </c>
       <c r="I153" t="str">
-        <f>VLOOKUP(B153,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8d/Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg/220px-Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B153,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/16/Sochi_Autodrom%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg/220px-Sochi_Autodrom%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
@@ -5900,11 +5900,11 @@
         <v>76</v>
       </c>
       <c r="H154" t="str">
-        <f>VLOOKUP(B154,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B154,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/5/54/Spa-Francorchamps_of_Belgium.svg/260px-Spa-Francorchamps_of_Belgium.svg.png</v>
       </c>
       <c r="I154" t="str">
-        <f>VLOOKUP(B154,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B154,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/77/Circuit_de_Spa-Francorchamps%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Spa-Francorchamps%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -5931,11 +5931,11 @@
         <v>81</v>
       </c>
       <c r="H155" t="str">
-        <f>VLOOKUP(B155,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B155,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/ec/Suzuka_circuit_map--2005.svg/260px-Suzuka_circuit_map--2005.svg.png</v>
       </c>
       <c r="I155" t="str">
-        <f>VLOOKUP(B155,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B155,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/9a/Suzuka_International_Racing_Course%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg/220px-Suzuka_International_Racing_Course%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -5962,11 +5962,11 @@
         <v>90</v>
       </c>
       <c r="H156" t="str">
-        <f>VLOOKUP(B156,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B156,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f9/%C3%8Ele_Notre-Dame_%28Circuit_Gilles_Villeneuve%29.svg/280px-%C3%8Ele_Notre-Dame_%28Circuit_Gilles_Villeneuve%29.svg.png</v>
       </c>
       <c r="I156" t="str">
-        <f>VLOOKUP(B156,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B156,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/3/38/F1_1978_circuit_ile_notre_dame.png/220px-F1_1978_circuit_ile_notre_dame.png</v>
       </c>
     </row>
@@ -5993,12 +5993,12 @@
         <v>95</v>
       </c>
       <c r="H157" t="str">
-        <f>VLOOKUP(B157,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/4c/Losail.svg/250px-Losail.svg.png</v>
+        <f>VLOOKUP(B157,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/b0/Yas_Marina_Circuit.png/250px-Yas_Marina_Circuit.png</v>
       </c>
       <c r="I157" t="str">
-        <f>VLOOKUP(B157,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://www.racefans.net/wp-content/uploads/2021/07/racefansdotnet-21-07-24-21-06-40-1.jpg</v>
+        <f>VLOOKUP(B157,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e1/Yas_Marina_Circuit%2C_October_12%2C_2018_SkySat_%28cropped%29.jpg/220px-Yas_Marina_Circuit%2C_October_12%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
@@ -6024,11 +6024,11 @@
         <v>11</v>
       </c>
       <c r="H158" t="str">
-        <f>VLOOKUP(B158,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B158,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0a/Albert_Park_Circuit_2021.svg/220px-Albert_Park_Circuit_2021.svg.png</v>
       </c>
       <c r="I158" t="str">
-        <f>VLOOKUP(B158,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B158,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8e/Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -6055,12 +6055,12 @@
         <v>114</v>
       </c>
       <c r="H159" t="str">
-        <f>VLOOKUP(B159,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0a/Albert_Park_Circuit_2021.svg/220px-Albert_Park_Circuit_2021.svg.png</v>
+        <f>VLOOKUP(B159,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/a/a5/Austin_circuit.svg/250px-Austin_circuit.svg.png</v>
       </c>
       <c r="I159" t="str">
-        <f>VLOOKUP(B159,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8e/Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B159,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/78/Circuit_of_the_Americas%2C_April_22%2C_2018_SkySat_%28cropped2%29.jpg/220px-Circuit_of_the_Americas%2C_April_22%2C_2018_SkySat_%28cropped2%29.jpg</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
@@ -6086,11 +6086,11 @@
         <v>16</v>
       </c>
       <c r="H160" t="str">
-        <f>VLOOKUP(B160,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B160,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/en/thumb/d/d1/Bahrain_International_Circuit_logo.png/200px-Bahrain_International_Circuit_logo.png</v>
       </c>
       <c r="I160" t="str">
-        <f>VLOOKUP(B160,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B160,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bc/Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg/220px-Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -6117,12 +6117,12 @@
         <v>134</v>
       </c>
       <c r="H161" t="str">
-        <f>VLOOKUP(B161,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/en/thumb/d/d1/Bahrain_International_Circuit_logo.png/200px-Bahrain_International_Circuit_logo.png</v>
+        <f>VLOOKUP(B161,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f1/Baku_Formula_One_circuit_map.svg/300px-Baku_Formula_One_circuit_map.svg.png</v>
       </c>
       <c r="I161" t="str">
-        <f>VLOOKUP(B161,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bc/Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg/220px-Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B161,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/76/Baku-F1-Street-Circuit-Openstreetmaps-rev1.png/220px-Baku-F1-Street-Circuit-Openstreetmaps-rev1.png</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
@@ -6148,11 +6148,11 @@
         <v>21</v>
       </c>
       <c r="H162" t="str">
-        <f>VLOOKUP(B162,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B162,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/87/Circuit_de_Catalunya_moto_2021.svg/250px-Circuit_de_Catalunya_moto_2021.svg.png</v>
       </c>
       <c r="I162" t="str">
-        <f>VLOOKUP(B162,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B162,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e7/Circuit_de_Barcelona-Catalunya%2C_April_19%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Barcelona-Catalunya%2C_April_19%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -6179,11 +6179,11 @@
         <v>26</v>
       </c>
       <c r="H163" t="str">
-        <f>VLOOKUP(B163,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B163,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e5/Hockenheim2012.svg/220px-Hockenheim2012.svg.png</v>
       </c>
       <c r="I163" t="str">
-        <f>VLOOKUP(B163,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B163,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/41/Hockenheimring%2C_April_29%2C_2018_SkySat_%28crop%29.jpg/220px-Hockenheimring%2C_April_29%2C_2018_SkySat_%28crop%29.jpg</v>
       </c>
     </row>
@@ -6210,11 +6210,11 @@
         <v>31</v>
       </c>
       <c r="H164" t="str">
-        <f>VLOOKUP(B164,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B164,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/91/Hungaroring.svg/260px-Hungaroring.svg.png</v>
       </c>
       <c r="I164" t="str">
-        <f>VLOOKUP(B164,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B164,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/a/aa/Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg/220px-Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -6241,11 +6241,11 @@
         <v>36</v>
       </c>
       <c r="H165" t="str">
-        <f>VLOOKUP(B165,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B165,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/cf/Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace_%28AKA_Interlagos%29_track_map.svg/260px-Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace_%28AKA_Interlagos%29_track_map.svg.png</v>
       </c>
       <c r="I165" t="str">
-        <f>VLOOKUP(B165,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B165,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/70/Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace%2C_July_3%2C_2018_SkySat_%28cropped%29.jpg/220px-Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace%2C_July_3%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -6272,11 +6272,11 @@
         <v>46</v>
       </c>
       <c r="H166" t="str">
-        <f>VLOOKUP(B166,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B166,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/17/Planned_2023_Marina_Bay_Street_Circuit_layout.png/220px-Planned_2023_Marina_Bay_Street_Circuit_layout.png</v>
       </c>
       <c r="I166" t="str">
-        <f>VLOOKUP(B166,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B166,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f0/1_singapore_f1_night_race_2012_city_skyline.jpg/240px-1_singapore_f1_night_race_2012_city_skyline.jpg</v>
       </c>
     </row>
@@ -6303,11 +6303,11 @@
         <v>51</v>
       </c>
       <c r="H167" t="str">
-        <f>VLOOKUP(B167,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B167,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/3/36/Monte_Carlo_Formula_1_track_map.svg/250px-Monte_Carlo_Formula_1_track_map.svg.png</v>
       </c>
       <c r="I167" t="str">
-        <f>VLOOKUP(B167,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B167,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/c7/Circuit_de_Monaco%2C_April_1%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Monaco%2C_April_1%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -6334,11 +6334,11 @@
         <v>56</v>
       </c>
       <c r="H168" t="str">
-        <f>VLOOKUP(B168,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B168,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
       </c>
       <c r="I168" t="str">
-        <f>VLOOKUP(B168,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B168,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -6365,12 +6365,12 @@
         <v>119</v>
       </c>
       <c r="H169" t="str">
-        <f>VLOOKUP(B169,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
+        <f>VLOOKUP(B169,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/9c/%C3%96sterreichring-A1Ring.svg/400px-%C3%96sterreichring-A1Ring.svg.png</v>
       </c>
       <c r="I169" t="str">
-        <f>VLOOKUP(B169,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B169,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/cb/Luftaufnahme_%28c%29Red_Bull_Ring.jpg/600px-Luftaufnahme_%28c%29Red_Bull_Ring.jpg</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
@@ -6396,12 +6396,12 @@
         <v>139</v>
       </c>
       <c r="H170" t="str">
-        <f>VLOOKUP(B170,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
+        <f>VLOOKUP(B170,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f2/Le_Castellet_circuit_map_Formula_One_2019_and_2021_with_corner_names_English_19_07_2021.svg/300px-Le_Castellet_circuit_map_Formula_One_2019_and_2021_with_corner_names_English_19_07_2021.svg.png</v>
       </c>
       <c r="I170" t="str">
-        <f>VLOOKUP(B170,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B170,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/5/59/Circuit_Paul_Ricard%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/250px-Circuit_Paul_Ricard%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
@@ -6427,12 +6427,12 @@
         <v>129</v>
       </c>
       <c r="H171" t="str">
-        <f>VLOOKUP(B171,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
+        <f>VLOOKUP(B171,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/c6/Autodromo_Hermanos_Rodriguez_%28Formula_E_Layout_2023%29.png/250px-Autodromo_Hermanos_Rodriguez_%28Formula_E_Layout_2023%29.png</v>
       </c>
       <c r="I171" t="str">
-        <f>VLOOKUP(B171,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B171,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f6/Aut%C3%B3dromo_Hermanos_Rodr%C3%ADguez%2C_June_4%2C_2018_SkySat_%28cropped%29.jpg/220px-Aut%C3%B3dromo_Hermanos_Rodr%C3%ADguez%2C_June_4%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
@@ -6458,11 +6458,11 @@
         <v>66</v>
       </c>
       <c r="H172" t="str">
-        <f>VLOOKUP(B172,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B172,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/14/Shanghai_International_Racing_Circuit_track_map.svg/250px-Shanghai_International_Racing_Circuit_track_map.svg.png</v>
       </c>
       <c r="I172" t="str">
-        <f>VLOOKUP(B172,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B172,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/d/d6/Shanghai_International_Circuit%2C_April_7%2C_2018_SkySat_%28rotated%29.jpg/220px-Shanghai_International_Circuit%2C_April_7%2C_2018_SkySat_%28rotated%29.jpg</v>
       </c>
     </row>
@@ -6489,11 +6489,11 @@
         <v>71</v>
       </c>
       <c r="H173" t="str">
-        <f>VLOOKUP(B173,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B173,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bd/Silverstone_Circuit_2020.png/250px-Silverstone_Circuit_2020.png</v>
       </c>
       <c r="I173" t="str">
-        <f>VLOOKUP(B173,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B173,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8d/Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg/220px-Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -6520,12 +6520,12 @@
         <v>124</v>
       </c>
       <c r="H174" t="str">
-        <f>VLOOKUP(B174,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bd/Silverstone_Circuit_2020.png/250px-Silverstone_Circuit_2020.png</v>
+        <f>VLOOKUP(B174,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/d/d3/Circuit_Sochi.svg/250px-Circuit_Sochi.svg.png</v>
       </c>
       <c r="I174" t="str">
-        <f>VLOOKUP(B174,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8d/Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg/220px-Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B174,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/16/Sochi_Autodrom%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg/220px-Sochi_Autodrom%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
@@ -6551,11 +6551,11 @@
         <v>76</v>
       </c>
       <c r="H175" t="str">
-        <f>VLOOKUP(B175,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B175,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/5/54/Spa-Francorchamps_of_Belgium.svg/260px-Spa-Francorchamps_of_Belgium.svg.png</v>
       </c>
       <c r="I175" t="str">
-        <f>VLOOKUP(B175,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B175,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/77/Circuit_de_Spa-Francorchamps%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Spa-Francorchamps%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -6582,11 +6582,11 @@
         <v>81</v>
       </c>
       <c r="H176" t="str">
-        <f>VLOOKUP(B176,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B176,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/ec/Suzuka_circuit_map--2005.svg/260px-Suzuka_circuit_map--2005.svg.png</v>
       </c>
       <c r="I176" t="str">
-        <f>VLOOKUP(B176,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B176,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/9a/Suzuka_International_Racing_Course%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg/220px-Suzuka_International_Racing_Course%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -6613,11 +6613,11 @@
         <v>90</v>
       </c>
       <c r="H177" t="str">
-        <f>VLOOKUP(B177,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B177,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f9/%C3%8Ele_Notre-Dame_%28Circuit_Gilles_Villeneuve%29.svg/280px-%C3%8Ele_Notre-Dame_%28Circuit_Gilles_Villeneuve%29.svg.png</v>
       </c>
       <c r="I177" t="str">
-        <f>VLOOKUP(B177,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B177,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/3/38/F1_1978_circuit_ile_notre_dame.png/220px-F1_1978_circuit_ile_notre_dame.png</v>
       </c>
     </row>
@@ -6644,12 +6644,12 @@
         <v>95</v>
       </c>
       <c r="H178" t="str">
-        <f>VLOOKUP(B178,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/4c/Losail.svg/250px-Losail.svg.png</v>
+        <f>VLOOKUP(B178,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/b0/Yas_Marina_Circuit.png/250px-Yas_Marina_Circuit.png</v>
       </c>
       <c r="I178" t="str">
-        <f>VLOOKUP(B178,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://www.racefans.net/wp-content/uploads/2021/07/racefansdotnet-21-07-24-21-06-40-1.jpg</v>
+        <f>VLOOKUP(B178,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e1/Yas_Marina_Circuit%2C_October_12%2C_2018_SkySat_%28cropped%29.jpg/220px-Yas_Marina_Circuit%2C_October_12%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
@@ -6675,11 +6675,11 @@
         <v>11</v>
       </c>
       <c r="H179" t="str">
-        <f>VLOOKUP(B179,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B179,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0a/Albert_Park_Circuit_2021.svg/220px-Albert_Park_Circuit_2021.svg.png</v>
       </c>
       <c r="I179" t="str">
-        <f>VLOOKUP(B179,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B179,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8e/Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -6706,12 +6706,12 @@
         <v>114</v>
       </c>
       <c r="H180" t="str">
-        <f>VLOOKUP(B180,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0a/Albert_Park_Circuit_2021.svg/220px-Albert_Park_Circuit_2021.svg.png</v>
+        <f>VLOOKUP(B180,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/a/a5/Austin_circuit.svg/250px-Austin_circuit.svg.png</v>
       </c>
       <c r="I180" t="str">
-        <f>VLOOKUP(B180,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8e/Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B180,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/78/Circuit_of_the_Americas%2C_April_22%2C_2018_SkySat_%28cropped2%29.jpg/220px-Circuit_of_the_Americas%2C_April_22%2C_2018_SkySat_%28cropped2%29.jpg</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
@@ -6737,11 +6737,11 @@
         <v>16</v>
       </c>
       <c r="H181" t="str">
-        <f>VLOOKUP(B181,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B181,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/en/thumb/d/d1/Bahrain_International_Circuit_logo.png/200px-Bahrain_International_Circuit_logo.png</v>
       </c>
       <c r="I181" t="str">
-        <f>VLOOKUP(B181,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B181,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bc/Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg/220px-Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -6768,12 +6768,12 @@
         <v>134</v>
       </c>
       <c r="H182" t="str">
-        <f>VLOOKUP(B182,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/en/thumb/d/d1/Bahrain_International_Circuit_logo.png/200px-Bahrain_International_Circuit_logo.png</v>
+        <f>VLOOKUP(B182,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f1/Baku_Formula_One_circuit_map.svg/300px-Baku_Formula_One_circuit_map.svg.png</v>
       </c>
       <c r="I182" t="str">
-        <f>VLOOKUP(B182,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bc/Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg/220px-Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B182,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/76/Baku-F1-Street-Circuit-Openstreetmaps-rev1.png/220px-Baku-F1-Street-Circuit-Openstreetmaps-rev1.png</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
@@ -6799,11 +6799,11 @@
         <v>21</v>
       </c>
       <c r="H183" t="str">
-        <f>VLOOKUP(B183,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B183,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/87/Circuit_de_Catalunya_moto_2021.svg/250px-Circuit_de_Catalunya_moto_2021.svg.png</v>
       </c>
       <c r="I183" t="str">
-        <f>VLOOKUP(B183,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B183,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e7/Circuit_de_Barcelona-Catalunya%2C_April_19%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Barcelona-Catalunya%2C_April_19%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -6830,11 +6830,11 @@
         <v>26</v>
       </c>
       <c r="H184" t="str">
-        <f>VLOOKUP(B184,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B184,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e5/Hockenheim2012.svg/220px-Hockenheim2012.svg.png</v>
       </c>
       <c r="I184" t="str">
-        <f>VLOOKUP(B184,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B184,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/41/Hockenheimring%2C_April_29%2C_2018_SkySat_%28crop%29.jpg/220px-Hockenheimring%2C_April_29%2C_2018_SkySat_%28crop%29.jpg</v>
       </c>
     </row>
@@ -6861,11 +6861,11 @@
         <v>31</v>
       </c>
       <c r="H185" t="str">
-        <f>VLOOKUP(B185,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B185,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/91/Hungaroring.svg/260px-Hungaroring.svg.png</v>
       </c>
       <c r="I185" t="str">
-        <f>VLOOKUP(B185,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B185,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/a/aa/Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg/220px-Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -6892,11 +6892,11 @@
         <v>36</v>
       </c>
       <c r="H186" t="str">
-        <f>VLOOKUP(B186,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B186,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/cf/Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace_%28AKA_Interlagos%29_track_map.svg/260px-Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace_%28AKA_Interlagos%29_track_map.svg.png</v>
       </c>
       <c r="I186" t="str">
-        <f>VLOOKUP(B186,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B186,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/70/Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace%2C_July_3%2C_2018_SkySat_%28cropped%29.jpg/220px-Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace%2C_July_3%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -6923,11 +6923,11 @@
         <v>46</v>
       </c>
       <c r="H187" t="str">
-        <f>VLOOKUP(B187,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B187,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/17/Planned_2023_Marina_Bay_Street_Circuit_layout.png/220px-Planned_2023_Marina_Bay_Street_Circuit_layout.png</v>
       </c>
       <c r="I187" t="str">
-        <f>VLOOKUP(B187,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B187,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f0/1_singapore_f1_night_race_2012_city_skyline.jpg/240px-1_singapore_f1_night_race_2012_city_skyline.jpg</v>
       </c>
     </row>
@@ -6954,11 +6954,11 @@
         <v>51</v>
       </c>
       <c r="H188" t="str">
-        <f>VLOOKUP(B188,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B188,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/3/36/Monte_Carlo_Formula_1_track_map.svg/250px-Monte_Carlo_Formula_1_track_map.svg.png</v>
       </c>
       <c r="I188" t="str">
-        <f>VLOOKUP(B188,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B188,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/c7/Circuit_de_Monaco%2C_April_1%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Monaco%2C_April_1%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -6985,11 +6985,11 @@
         <v>56</v>
       </c>
       <c r="H189" t="str">
-        <f>VLOOKUP(B189,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B189,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
       </c>
       <c r="I189" t="str">
-        <f>VLOOKUP(B189,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B189,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -7016,12 +7016,12 @@
         <v>119</v>
       </c>
       <c r="H190" t="str">
-        <f>VLOOKUP(B190,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
+        <f>VLOOKUP(B190,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/9c/%C3%96sterreichring-A1Ring.svg/400px-%C3%96sterreichring-A1Ring.svg.png</v>
       </c>
       <c r="I190" t="str">
-        <f>VLOOKUP(B190,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B190,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/cb/Luftaufnahme_%28c%29Red_Bull_Ring.jpg/600px-Luftaufnahme_%28c%29Red_Bull_Ring.jpg</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.25">
@@ -7047,12 +7047,12 @@
         <v>139</v>
       </c>
       <c r="H191" t="str">
-        <f>VLOOKUP(B191,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
+        <f>VLOOKUP(B191,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f2/Le_Castellet_circuit_map_Formula_One_2019_and_2021_with_corner_names_English_19_07_2021.svg/300px-Le_Castellet_circuit_map_Formula_One_2019_and_2021_with_corner_names_English_19_07_2021.svg.png</v>
       </c>
       <c r="I191" t="str">
-        <f>VLOOKUP(B191,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B191,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/5/59/Circuit_Paul_Ricard%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/250px-Circuit_Paul_Ricard%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.25">
@@ -7078,12 +7078,12 @@
         <v>129</v>
       </c>
       <c r="H192" t="str">
-        <f>VLOOKUP(B192,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
+        <f>VLOOKUP(B192,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/c6/Autodromo_Hermanos_Rodriguez_%28Formula_E_Layout_2023%29.png/250px-Autodromo_Hermanos_Rodriguez_%28Formula_E_Layout_2023%29.png</v>
       </c>
       <c r="I192" t="str">
-        <f>VLOOKUP(B192,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B192,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f6/Aut%C3%B3dromo_Hermanos_Rodr%C3%ADguez%2C_June_4%2C_2018_SkySat_%28cropped%29.jpg/220px-Aut%C3%B3dromo_Hermanos_Rodr%C3%ADguez%2C_June_4%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
@@ -7109,11 +7109,11 @@
         <v>66</v>
       </c>
       <c r="H193" t="str">
-        <f>VLOOKUP(B193,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B193,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/14/Shanghai_International_Racing_Circuit_track_map.svg/250px-Shanghai_International_Racing_Circuit_track_map.svg.png</v>
       </c>
       <c r="I193" t="str">
-        <f>VLOOKUP(B193,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B193,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/d/d6/Shanghai_International_Circuit%2C_April_7%2C_2018_SkySat_%28rotated%29.jpg/220px-Shanghai_International_Circuit%2C_April_7%2C_2018_SkySat_%28rotated%29.jpg</v>
       </c>
     </row>
@@ -7140,11 +7140,11 @@
         <v>71</v>
       </c>
       <c r="H194" t="str">
-        <f>VLOOKUP(B194,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B194,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bd/Silverstone_Circuit_2020.png/250px-Silverstone_Circuit_2020.png</v>
       </c>
       <c r="I194" t="str">
-        <f>VLOOKUP(B194,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B194,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8d/Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg/220px-Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -7171,12 +7171,12 @@
         <v>124</v>
       </c>
       <c r="H195" t="str">
-        <f>VLOOKUP(B195,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bd/Silverstone_Circuit_2020.png/250px-Silverstone_Circuit_2020.png</v>
+        <f>VLOOKUP(B195,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/d/d3/Circuit_Sochi.svg/250px-Circuit_Sochi.svg.png</v>
       </c>
       <c r="I195" t="str">
-        <f>VLOOKUP(B195,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8d/Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg/220px-Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B195,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/16/Sochi_Autodrom%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg/220px-Sochi_Autodrom%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.25">
@@ -7202,11 +7202,11 @@
         <v>76</v>
       </c>
       <c r="H196" t="str">
-        <f>VLOOKUP(B196,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B196,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/5/54/Spa-Francorchamps_of_Belgium.svg/260px-Spa-Francorchamps_of_Belgium.svg.png</v>
       </c>
       <c r="I196" t="str">
-        <f>VLOOKUP(B196,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B196,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/77/Circuit_de_Spa-Francorchamps%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Spa-Francorchamps%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -7233,11 +7233,11 @@
         <v>81</v>
       </c>
       <c r="H197" t="str">
-        <f>VLOOKUP(B197,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B197,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/ec/Suzuka_circuit_map--2005.svg/260px-Suzuka_circuit_map--2005.svg.png</v>
       </c>
       <c r="I197" t="str">
-        <f>VLOOKUP(B197,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B197,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/9a/Suzuka_International_Racing_Course%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg/220px-Suzuka_International_Racing_Course%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -7264,11 +7264,11 @@
         <v>90</v>
       </c>
       <c r="H198" t="str">
-        <f>VLOOKUP(B198,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B198,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f9/%C3%8Ele_Notre-Dame_%28Circuit_Gilles_Villeneuve%29.svg/280px-%C3%8Ele_Notre-Dame_%28Circuit_Gilles_Villeneuve%29.svg.png</v>
       </c>
       <c r="I198" t="str">
-        <f>VLOOKUP(B198,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B198,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/3/38/F1_1978_circuit_ile_notre_dame.png/220px-F1_1978_circuit_ile_notre_dame.png</v>
       </c>
     </row>
@@ -7295,12 +7295,12 @@
         <v>95</v>
       </c>
       <c r="H199" t="str">
-        <f>VLOOKUP(B199,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/4c/Losail.svg/250px-Losail.svg.png</v>
+        <f>VLOOKUP(B199,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/b0/Yas_Marina_Circuit.png/250px-Yas_Marina_Circuit.png</v>
       </c>
       <c r="I199" t="str">
-        <f>VLOOKUP(B199,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://www.racefans.net/wp-content/uploads/2021/07/racefansdotnet-21-07-24-21-06-40-1.jpg</v>
+        <f>VLOOKUP(B199,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e1/Yas_Marina_Circuit%2C_October_12%2C_2018_SkySat_%28cropped%29.jpg/220px-Yas_Marina_Circuit%2C_October_12%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.25">
@@ -7326,11 +7326,11 @@
         <v>16</v>
       </c>
       <c r="H200" t="str">
-        <f>VLOOKUP(B200,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B200,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/en/thumb/d/d1/Bahrain_International_Circuit_logo.png/200px-Bahrain_International_Circuit_logo.png</v>
       </c>
       <c r="I200" t="str">
-        <f>VLOOKUP(B200,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B200,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bc/Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg/220px-Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -7357,11 +7357,11 @@
         <v>21</v>
       </c>
       <c r="H201" t="str">
-        <f>VLOOKUP(B201,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B201,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/87/Circuit_de_Catalunya_moto_2021.svg/250px-Circuit_de_Catalunya_moto_2021.svg.png</v>
       </c>
       <c r="I201" t="str">
-        <f>VLOOKUP(B201,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B201,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e7/Circuit_de_Barcelona-Catalunya%2C_April_19%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Barcelona-Catalunya%2C_April_19%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -7388,11 +7388,11 @@
         <v>31</v>
       </c>
       <c r="H202" t="str">
-        <f>VLOOKUP(B202,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B202,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/91/Hungaroring.svg/260px-Hungaroring.svg.png</v>
       </c>
       <c r="I202" t="str">
-        <f>VLOOKUP(B202,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B202,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/a/aa/Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg/220px-Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -7419,12 +7419,12 @@
         <v>143</v>
       </c>
       <c r="H203" t="str">
-        <f>VLOOKUP(B203,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/91/Hungaroring.svg/260px-Hungaroring.svg.png</v>
+        <f>VLOOKUP(B203,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/2/22/Imola_2009.svg/300px-Imola_2009.svg.png</v>
       </c>
       <c r="I203" t="str">
-        <f>VLOOKUP(B203,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/a/aa/Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg/220px-Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B203,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/2/24/Imola2007.jpg/200px-Imola2007.jpg</v>
       </c>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
@@ -7450,11 +7450,11 @@
         <v>41</v>
       </c>
       <c r="H204" t="str">
-        <f>VLOOKUP(B204,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B204,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/en/7/7c/Istanbulpark.png</v>
       </c>
       <c r="I204" t="str">
-        <f>VLOOKUP(B204,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B204,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/90/Istanbul_Park_aerial.jpg/270px-Istanbul_Park_aerial.jpg</v>
       </c>
     </row>
@@ -7481,11 +7481,11 @@
         <v>56</v>
       </c>
       <c r="H205" t="str">
-        <f>VLOOKUP(B205,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B205,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
       </c>
       <c r="I205" t="str">
-        <f>VLOOKUP(B205,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B205,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -7512,12 +7512,12 @@
         <v>147</v>
       </c>
       <c r="H206" t="str">
-        <f>VLOOKUP(B206,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
+        <f>VLOOKUP(B206,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/3/38/Mugello_Racing_Circuit_track_map_15_turns.svg/250px-Mugello_Racing_Circuit_track_map_15_turns.svg.png</v>
       </c>
       <c r="I206" t="str">
-        <f>VLOOKUP(B206,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B206,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/60/Partenza_del_Gran_Premio_d%27Italia_TIM_2011.jpg/220px-Partenza_del_Gran_Premio_d%27Italia_TIM_2011.jpg</v>
       </c>
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.25">
@@ -7543,12 +7543,12 @@
         <v>109</v>
       </c>
       <c r="H207" t="str">
-        <f>VLOOKUP(B207,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
+        <f>VLOOKUP(B207,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/76/N%C3%BCrburgring_-_Grand-Prix-Strecke.svg/230px-N%C3%BCrburgring_-_Grand-Prix-Strecke.svg.png</v>
       </c>
       <c r="I207" t="str">
-        <f>VLOOKUP(B207,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B207,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/4c/Panorama_N%C3%BCrburgring_Haupteingang_2010.jpg/530px-Panorama_N%C3%BCrburgring_Haupteingang_2010.jpg</v>
       </c>
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.25">
@@ -7574,12 +7574,12 @@
         <v>152</v>
       </c>
       <c r="H208" t="str">
-        <f>VLOOKUP(B208,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
+        <f>VLOOKUP(B208,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0a/Aut%C3%B3dromo_do_Algarve_F1_Sectors.svg/250px-Aut%C3%B3dromo_do_Algarve_F1_Sectors.svg.png</v>
       </c>
       <c r="I208" t="str">
-        <f>VLOOKUP(B208,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B208,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/2/2e/Aut%C3%B3dromo_Internacional_do_Algarve_%282012-09-23%29%2C_by_Klugschnacker_in_Wikipedia_%2825%29.JPG/220px-Aut%C3%B3dromo_Internacional_do_Algarve_%282012-09-23%29%2C_by_Klugschnacker_in_Wikipedia_%2825%29.JPG</v>
       </c>
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.25">
@@ -7605,12 +7605,12 @@
         <v>119</v>
       </c>
       <c r="H209" t="str">
-        <f>VLOOKUP(B209,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
+        <f>VLOOKUP(B209,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/9c/%C3%96sterreichring-A1Ring.svg/400px-%C3%96sterreichring-A1Ring.svg.png</v>
       </c>
       <c r="I209" t="str">
-        <f>VLOOKUP(B209,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B209,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/cb/Luftaufnahme_%28c%29Red_Bull_Ring.jpg/600px-Luftaufnahme_%28c%29Red_Bull_Ring.jpg</v>
       </c>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.25">
@@ -7636,11 +7636,11 @@
         <v>71</v>
       </c>
       <c r="H210" t="str">
-        <f>VLOOKUP(B210,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B210,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bd/Silverstone_Circuit_2020.png/250px-Silverstone_Circuit_2020.png</v>
       </c>
       <c r="I210" t="str">
-        <f>VLOOKUP(B210,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B210,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8d/Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg/220px-Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -7667,12 +7667,12 @@
         <v>124</v>
       </c>
       <c r="H211" t="str">
-        <f>VLOOKUP(B211,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bd/Silverstone_Circuit_2020.png/250px-Silverstone_Circuit_2020.png</v>
+        <f>VLOOKUP(B211,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/d/d3/Circuit_Sochi.svg/250px-Circuit_Sochi.svg.png</v>
       </c>
       <c r="I211" t="str">
-        <f>VLOOKUP(B211,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8d/Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg/220px-Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B211,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/16/Sochi_Autodrom%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg/220px-Sochi_Autodrom%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
@@ -7698,11 +7698,11 @@
         <v>76</v>
       </c>
       <c r="H212" t="str">
-        <f>VLOOKUP(B212,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B212,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/5/54/Spa-Francorchamps_of_Belgium.svg/260px-Spa-Francorchamps_of_Belgium.svg.png</v>
       </c>
       <c r="I212" t="str">
-        <f>VLOOKUP(B212,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B212,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/77/Circuit_de_Spa-Francorchamps%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Spa-Francorchamps%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -7729,12 +7729,12 @@
         <v>95</v>
       </c>
       <c r="H213" t="str">
-        <f>VLOOKUP(B213,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/4c/Losail.svg/250px-Losail.svg.png</v>
+        <f>VLOOKUP(B213,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/b0/Yas_Marina_Circuit.png/250px-Yas_Marina_Circuit.png</v>
       </c>
       <c r="I213" t="str">
-        <f>VLOOKUP(B213,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://www.racefans.net/wp-content/uploads/2021/07/racefansdotnet-21-07-24-21-06-40-1.jpg</v>
+        <f>VLOOKUP(B213,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e1/Yas_Marina_Circuit%2C_October_12%2C_2018_SkySat_%28cropped%29.jpg/220px-Yas_Marina_Circuit%2C_October_12%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
@@ -7760,12 +7760,12 @@
         <v>114</v>
       </c>
       <c r="H214" t="str">
-        <f>VLOOKUP(B214,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0a/Albert_Park_Circuit_2021.svg/220px-Albert_Park_Circuit_2021.svg.png</v>
+        <f>VLOOKUP(B214,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/a/a5/Austin_circuit.svg/250px-Austin_circuit.svg.png</v>
       </c>
       <c r="I214" t="str">
-        <f>VLOOKUP(B214,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8e/Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B214,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/78/Circuit_of_the_Americas%2C_April_22%2C_2018_SkySat_%28cropped2%29.jpg/220px-Circuit_of_the_Americas%2C_April_22%2C_2018_SkySat_%28cropped2%29.jpg</v>
       </c>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.25">
@@ -7791,11 +7791,11 @@
         <v>16</v>
       </c>
       <c r="H215" t="str">
-        <f>VLOOKUP(B215,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B215,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/en/thumb/d/d1/Bahrain_International_Circuit_logo.png/200px-Bahrain_International_Circuit_logo.png</v>
       </c>
       <c r="I215" t="str">
-        <f>VLOOKUP(B215,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B215,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bc/Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg/220px-Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -7822,12 +7822,12 @@
         <v>134</v>
       </c>
       <c r="H216" t="str">
-        <f>VLOOKUP(B216,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/en/thumb/d/d1/Bahrain_International_Circuit_logo.png/200px-Bahrain_International_Circuit_logo.png</v>
+        <f>VLOOKUP(B216,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f1/Baku_Formula_One_circuit_map.svg/300px-Baku_Formula_One_circuit_map.svg.png</v>
       </c>
       <c r="I216" t="str">
-        <f>VLOOKUP(B216,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bc/Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg/220px-Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B216,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/76/Baku-F1-Street-Circuit-Openstreetmaps-rev1.png/220px-Baku-F1-Street-Circuit-Openstreetmaps-rev1.png</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.25">
@@ -7853,11 +7853,11 @@
         <v>21</v>
       </c>
       <c r="H217" t="str">
-        <f>VLOOKUP(B217,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B217,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/87/Circuit_de_Catalunya_moto_2021.svg/250px-Circuit_de_Catalunya_moto_2021.svg.png</v>
       </c>
       <c r="I217" t="str">
-        <f>VLOOKUP(B217,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B217,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e7/Circuit_de_Barcelona-Catalunya%2C_April_19%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Barcelona-Catalunya%2C_April_19%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -7884,11 +7884,11 @@
         <v>31</v>
       </c>
       <c r="H218" t="str">
-        <f>VLOOKUP(B218,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B218,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/91/Hungaroring.svg/260px-Hungaroring.svg.png</v>
       </c>
       <c r="I218" t="str">
-        <f>VLOOKUP(B218,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B218,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/a/aa/Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg/220px-Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -7915,12 +7915,12 @@
         <v>143</v>
       </c>
       <c r="H219" t="str">
-        <f>VLOOKUP(B219,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/91/Hungaroring.svg/260px-Hungaroring.svg.png</v>
+        <f>VLOOKUP(B219,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/2/22/Imola_2009.svg/300px-Imola_2009.svg.png</v>
       </c>
       <c r="I219" t="str">
-        <f>VLOOKUP(B219,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/a/aa/Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg/220px-Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B219,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/2/24/Imola2007.jpg/200px-Imola2007.jpg</v>
       </c>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.25">
@@ -7946,11 +7946,11 @@
         <v>36</v>
       </c>
       <c r="H220" t="str">
-        <f>VLOOKUP(B220,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B220,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/cf/Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace_%28AKA_Interlagos%29_track_map.svg/260px-Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace_%28AKA_Interlagos%29_track_map.svg.png</v>
       </c>
       <c r="I220" t="str">
-        <f>VLOOKUP(B220,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B220,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/70/Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace%2C_July_3%2C_2018_SkySat_%28cropped%29.jpg/220px-Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace%2C_July_3%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -7977,11 +7977,11 @@
         <v>41</v>
       </c>
       <c r="H221" t="str">
-        <f>VLOOKUP(B221,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B221,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/en/7/7c/Istanbulpark.png</v>
       </c>
       <c r="I221" t="str">
-        <f>VLOOKUP(B221,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B221,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/90/Istanbul_Park_aerial.jpg/270px-Istanbul_Park_aerial.jpg</v>
       </c>
     </row>
@@ -8008,12 +8008,12 @@
         <v>157</v>
       </c>
       <c r="H222" t="str">
-        <f>VLOOKUP(B222,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/en/7/7c/Istanbulpark.png</v>
+        <f>VLOOKUP(B222,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/4c/Jeddah_Street_Circuit_2021.svg/220px-Jeddah_Street_Circuit_2021.svg.png</v>
       </c>
       <c r="I222" t="str">
-        <f>VLOOKUP(B222,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/90/Istanbul_Park_aerial.jpg/270px-Istanbul_Park_aerial.jpg</v>
+        <f>VLOOKUP(B222,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://www.grandprix247.com/wp-content/uploads/2021/11/jeddah-circuit-15.jpg</v>
       </c>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.25">
@@ -8039,12 +8039,12 @@
         <v>162</v>
       </c>
       <c r="H223" t="str">
-        <f>VLOOKUP(B223,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/en/7/7c/Istanbulpark.png</v>
+        <f>VLOOKUP(B223,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/4c/Losail.svg/250px-Losail.svg.png</v>
       </c>
       <c r="I223" t="str">
-        <f>VLOOKUP(B223,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/90/Istanbul_Park_aerial.jpg/270px-Istanbul_Park_aerial.jpg</v>
+        <f>VLOOKUP(B223,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://www.racefans.net/wp-content/uploads/2021/07/racefansdotnet-21-07-24-21-06-40-1.jpg</v>
       </c>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.25">
@@ -8070,11 +8070,11 @@
         <v>51</v>
       </c>
       <c r="H224" t="str">
-        <f>VLOOKUP(B224,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B224,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/3/36/Monte_Carlo_Formula_1_track_map.svg/250px-Monte_Carlo_Formula_1_track_map.svg.png</v>
       </c>
       <c r="I224" t="str">
-        <f>VLOOKUP(B224,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B224,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/c7/Circuit_de_Monaco%2C_April_1%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Monaco%2C_April_1%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -8101,11 +8101,11 @@
         <v>56</v>
       </c>
       <c r="H225" t="str">
-        <f>VLOOKUP(B225,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B225,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
       </c>
       <c r="I225" t="str">
-        <f>VLOOKUP(B225,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B225,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -8132,12 +8132,12 @@
         <v>152</v>
       </c>
       <c r="H226" t="str">
-        <f>VLOOKUP(B226,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
+        <f>VLOOKUP(B226,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0a/Aut%C3%B3dromo_do_Algarve_F1_Sectors.svg/250px-Aut%C3%B3dromo_do_Algarve_F1_Sectors.svg.png</v>
       </c>
       <c r="I226" t="str">
-        <f>VLOOKUP(B226,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B226,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/2/2e/Aut%C3%B3dromo_Internacional_do_Algarve_%282012-09-23%29%2C_by_Klugschnacker_in_Wikipedia_%2825%29.JPG/220px-Aut%C3%B3dromo_Internacional_do_Algarve_%282012-09-23%29%2C_by_Klugschnacker_in_Wikipedia_%2825%29.JPG</v>
       </c>
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.25">
@@ -8163,12 +8163,12 @@
         <v>119</v>
       </c>
       <c r="H227" t="str">
-        <f>VLOOKUP(B227,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
+        <f>VLOOKUP(B227,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/9c/%C3%96sterreichring-A1Ring.svg/400px-%C3%96sterreichring-A1Ring.svg.png</v>
       </c>
       <c r="I227" t="str">
-        <f>VLOOKUP(B227,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B227,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/cb/Luftaufnahme_%28c%29Red_Bull_Ring.jpg/600px-Luftaufnahme_%28c%29Red_Bull_Ring.jpg</v>
       </c>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.25">
@@ -8194,12 +8194,12 @@
         <v>139</v>
       </c>
       <c r="H228" t="str">
-        <f>VLOOKUP(B228,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
+        <f>VLOOKUP(B228,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f2/Le_Castellet_circuit_map_Formula_One_2019_and_2021_with_corner_names_English_19_07_2021.svg/300px-Le_Castellet_circuit_map_Formula_One_2019_and_2021_with_corner_names_English_19_07_2021.svg.png</v>
       </c>
       <c r="I228" t="str">
-        <f>VLOOKUP(B228,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B228,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/5/59/Circuit_Paul_Ricard%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/250px-Circuit_Paul_Ricard%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.25">
@@ -8225,12 +8225,12 @@
         <v>129</v>
       </c>
       <c r="H229" t="str">
-        <f>VLOOKUP(B229,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
+        <f>VLOOKUP(B229,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/c6/Autodromo_Hermanos_Rodriguez_%28Formula_E_Layout_2023%29.png/250px-Autodromo_Hermanos_Rodriguez_%28Formula_E_Layout_2023%29.png</v>
       </c>
       <c r="I229" t="str">
-        <f>VLOOKUP(B229,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B229,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f6/Aut%C3%B3dromo_Hermanos_Rodr%C3%ADguez%2C_June_4%2C_2018_SkySat_%28cropped%29.jpg/220px-Aut%C3%B3dromo_Hermanos_Rodr%C3%ADguez%2C_June_4%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.25">
@@ -8256,11 +8256,11 @@
         <v>71</v>
       </c>
       <c r="H230" t="str">
-        <f>VLOOKUP(B230,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B230,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bd/Silverstone_Circuit_2020.png/250px-Silverstone_Circuit_2020.png</v>
       </c>
       <c r="I230" t="str">
-        <f>VLOOKUP(B230,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B230,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8d/Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg/220px-Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -8287,12 +8287,12 @@
         <v>124</v>
       </c>
       <c r="H231" t="str">
-        <f>VLOOKUP(B231,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bd/Silverstone_Circuit_2020.png/250px-Silverstone_Circuit_2020.png</v>
+        <f>VLOOKUP(B231,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/d/d3/Circuit_Sochi.svg/250px-Circuit_Sochi.svg.png</v>
       </c>
       <c r="I231" t="str">
-        <f>VLOOKUP(B231,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8d/Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg/220px-Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B231,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/16/Sochi_Autodrom%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg/220px-Sochi_Autodrom%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.25">
@@ -8318,11 +8318,11 @@
         <v>76</v>
       </c>
       <c r="H232" t="str">
-        <f>VLOOKUP(B232,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B232,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/5/54/Spa-Francorchamps_of_Belgium.svg/260px-Spa-Francorchamps_of_Belgium.svg.png</v>
       </c>
       <c r="I232" t="str">
-        <f>VLOOKUP(B232,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B232,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/77/Circuit_de_Spa-Francorchamps%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Spa-Francorchamps%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -8349,12 +8349,12 @@
         <v>95</v>
       </c>
       <c r="H233" t="str">
-        <f>VLOOKUP(B233,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/4c/Losail.svg/250px-Losail.svg.png</v>
+        <f>VLOOKUP(B233,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/b0/Yas_Marina_Circuit.png/250px-Yas_Marina_Circuit.png</v>
       </c>
       <c r="I233" t="str">
-        <f>VLOOKUP(B233,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://www.racefans.net/wp-content/uploads/2021/07/racefansdotnet-21-07-24-21-06-40-1.jpg</v>
+        <f>VLOOKUP(B233,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e1/Yas_Marina_Circuit%2C_October_12%2C_2018_SkySat_%28cropped%29.jpg/220px-Yas_Marina_Circuit%2C_October_12%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.25">
@@ -8380,11 +8380,11 @@
         <v>167</v>
       </c>
       <c r="H234" t="str">
-        <f>VLOOKUP(B234,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B234,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/78/Zandvoort_Circuit.png/250px-Zandvoort_Circuit.png</v>
       </c>
       <c r="I234" t="str">
-        <f>VLOOKUP(B234,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B234,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/49/Circuit_Park_Zandvoort_from_air_2016-08-24.jpg/220px-Circuit_Park_Zandvoort_from_air_2016-08-24.jpg</v>
       </c>
     </row>
@@ -8411,11 +8411,11 @@
         <v>11</v>
       </c>
       <c r="H235" t="str">
-        <f>VLOOKUP(B235,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B235,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0a/Albert_Park_Circuit_2021.svg/220px-Albert_Park_Circuit_2021.svg.png</v>
       </c>
       <c r="I235" t="str">
-        <f>VLOOKUP(B235,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B235,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8e/Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -8442,12 +8442,12 @@
         <v>114</v>
       </c>
       <c r="H236" t="str">
-        <f>VLOOKUP(B236,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0a/Albert_Park_Circuit_2021.svg/220px-Albert_Park_Circuit_2021.svg.png</v>
+        <f>VLOOKUP(B236,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/a/a5/Austin_circuit.svg/250px-Austin_circuit.svg.png</v>
       </c>
       <c r="I236" t="str">
-        <f>VLOOKUP(B236,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8e/Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Melbourne_Grand_Prix_Circuit%2C_March_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B236,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/78/Circuit_of_the_Americas%2C_April_22%2C_2018_SkySat_%28cropped2%29.jpg/220px-Circuit_of_the_Americas%2C_April_22%2C_2018_SkySat_%28cropped2%29.jpg</v>
       </c>
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.25">
@@ -8473,11 +8473,11 @@
         <v>16</v>
       </c>
       <c r="H237" t="str">
-        <f>VLOOKUP(B237,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B237,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/en/thumb/d/d1/Bahrain_International_Circuit_logo.png/200px-Bahrain_International_Circuit_logo.png</v>
       </c>
       <c r="I237" t="str">
-        <f>VLOOKUP(B237,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B237,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bc/Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg/220px-Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -8504,12 +8504,12 @@
         <v>134</v>
       </c>
       <c r="H238" t="str">
-        <f>VLOOKUP(B238,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/en/thumb/d/d1/Bahrain_International_Circuit_logo.png/200px-Bahrain_International_Circuit_logo.png</v>
+        <f>VLOOKUP(B238,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f1/Baku_Formula_One_circuit_map.svg/300px-Baku_Formula_One_circuit_map.svg.png</v>
       </c>
       <c r="I238" t="str">
-        <f>VLOOKUP(B238,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bc/Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg/220px-Bahrain_International_Circuit%2C_November_2%2C_2017_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B238,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/76/Baku-F1-Street-Circuit-Openstreetmaps-rev1.png/220px-Baku-F1-Street-Circuit-Openstreetmaps-rev1.png</v>
       </c>
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.25">
@@ -8535,11 +8535,11 @@
         <v>21</v>
       </c>
       <c r="H239" t="str">
-        <f>VLOOKUP(B239,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B239,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/87/Circuit_de_Catalunya_moto_2021.svg/250px-Circuit_de_Catalunya_moto_2021.svg.png</v>
       </c>
       <c r="I239" t="str">
-        <f>VLOOKUP(B239,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B239,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e7/Circuit_de_Barcelona-Catalunya%2C_April_19%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Barcelona-Catalunya%2C_April_19%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -8566,11 +8566,11 @@
         <v>31</v>
       </c>
       <c r="H240" t="str">
-        <f>VLOOKUP(B240,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B240,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/91/Hungaroring.svg/260px-Hungaroring.svg.png</v>
       </c>
       <c r="I240" t="str">
-        <f>VLOOKUP(B240,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B240,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/a/aa/Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg/220px-Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -8597,12 +8597,12 @@
         <v>143</v>
       </c>
       <c r="H241" t="str">
-        <f>VLOOKUP(B241,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/91/Hungaroring.svg/260px-Hungaroring.svg.png</v>
+        <f>VLOOKUP(B241,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/2/22/Imola_2009.svg/300px-Imola_2009.svg.png</v>
       </c>
       <c r="I241" t="str">
-        <f>VLOOKUP(B241,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/a/aa/Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg/220px-Hungaroring%2C_April_28%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B241,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/2/24/Imola2007.jpg/200px-Imola2007.jpg</v>
       </c>
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.25">
@@ -8628,11 +8628,11 @@
         <v>36</v>
       </c>
       <c r="H242" t="str">
-        <f>VLOOKUP(B242,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B242,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/cf/Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace_%28AKA_Interlagos%29_track_map.svg/260px-Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace_%28AKA_Interlagos%29_track_map.svg.png</v>
       </c>
       <c r="I242" t="str">
-        <f>VLOOKUP(B242,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B242,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/70/Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace%2C_July_3%2C_2018_SkySat_%28cropped%29.jpg/220px-Aut%C3%B3dromo_Jos%C3%A9_Carlos_Pace%2C_July_3%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -8659,12 +8659,12 @@
         <v>157</v>
       </c>
       <c r="H243" t="str">
-        <f>VLOOKUP(B243,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/en/7/7c/Istanbulpark.png</v>
+        <f>VLOOKUP(B243,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/4c/Jeddah_Street_Circuit_2021.svg/220px-Jeddah_Street_Circuit_2021.svg.png</v>
       </c>
       <c r="I243" t="str">
-        <f>VLOOKUP(B243,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/90/Istanbul_Park_aerial.jpg/270px-Istanbul_Park_aerial.jpg</v>
+        <f>VLOOKUP(B243,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://www.grandprix247.com/wp-content/uploads/2021/11/jeddah-circuit-15.jpg</v>
       </c>
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.25">
@@ -8690,11 +8690,11 @@
         <v>46</v>
       </c>
       <c r="H244" t="str">
-        <f>VLOOKUP(B244,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B244,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/17/Planned_2023_Marina_Bay_Street_Circuit_layout.png/220px-Planned_2023_Marina_Bay_Street_Circuit_layout.png</v>
       </c>
       <c r="I244" t="str">
-        <f>VLOOKUP(B244,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B244,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f0/1_singapore_f1_night_race_2012_city_skyline.jpg/240px-1_singapore_f1_night_race_2012_city_skyline.jpg</v>
       </c>
     </row>
@@ -8721,12 +8721,12 @@
         <v>171</v>
       </c>
       <c r="H245" t="str">
-        <f>VLOOKUP(B245,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/1/17/Planned_2023_Marina_Bay_Street_Circuit_layout.png/220px-Planned_2023_Marina_Bay_Street_Circuit_layout.png</v>
+        <f>VLOOKUP(B245,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/49/Hard_Rock_Stadium_Circuit_2022.svg/300px-Hard_Rock_Stadium_Circuit_2022.svg.png</v>
       </c>
       <c r="I245" t="str">
-        <f>VLOOKUP(B245,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f0/1_singapore_f1_night_race_2012_city_skyline.jpg/240px-1_singapore_f1_night_race_2012_city_skyline.jpg</v>
+        <f>VLOOKUP(B245,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://www.racefans.net/wp-content/uploads/2022/05/racefansdotnet-21-05-05-13-55-01-1.jpg</v>
       </c>
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.25">
@@ -8752,11 +8752,11 @@
         <v>51</v>
       </c>
       <c r="H246" t="str">
-        <f>VLOOKUP(B246,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B246,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/3/36/Monte_Carlo_Formula_1_track_map.svg/250px-Monte_Carlo_Formula_1_track_map.svg.png</v>
       </c>
       <c r="I246" t="str">
-        <f>VLOOKUP(B246,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B246,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/c7/Circuit_de_Monaco%2C_April_1%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Monaco%2C_April_1%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -8783,11 +8783,11 @@
         <v>56</v>
       </c>
       <c r="H247" t="str">
-        <f>VLOOKUP(B247,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B247,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
       </c>
       <c r="I247" t="str">
-        <f>VLOOKUP(B247,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B247,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -8814,12 +8814,12 @@
         <v>119</v>
       </c>
       <c r="H248" t="str">
-        <f>VLOOKUP(B248,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
+        <f>VLOOKUP(B248,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/9c/%C3%96sterreichring-A1Ring.svg/400px-%C3%96sterreichring-A1Ring.svg.png</v>
       </c>
       <c r="I248" t="str">
-        <f>VLOOKUP(B248,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B248,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/cb/Luftaufnahme_%28c%29Red_Bull_Ring.jpg/600px-Luftaufnahme_%28c%29Red_Bull_Ring.jpg</v>
       </c>
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.25">
@@ -8845,12 +8845,12 @@
         <v>139</v>
       </c>
       <c r="H249" t="str">
-        <f>VLOOKUP(B249,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
+        <f>VLOOKUP(B249,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f2/Le_Castellet_circuit_map_Formula_One_2019_and_2021_with_corner_names_English_19_07_2021.svg/300px-Le_Castellet_circuit_map_Formula_One_2019_and_2021_with_corner_names_English_19_07_2021.svg.png</v>
       </c>
       <c r="I249" t="str">
-        <f>VLOOKUP(B249,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B249,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/5/59/Circuit_Paul_Ricard%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/250px-Circuit_Paul_Ricard%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.25">
@@ -8876,12 +8876,12 @@
         <v>129</v>
       </c>
       <c r="H250" t="str">
-        <f>VLOOKUP(B250,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f8/Monza_track_map.svg/260px-Monza_track_map.svg.png</v>
+        <f>VLOOKUP(B250,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/c/c6/Autodromo_Hermanos_Rodriguez_%28Formula_E_Layout_2023%29.png/250px-Autodromo_Hermanos_Rodriguez_%28Formula_E_Layout_2023%29.png</v>
       </c>
       <c r="I250" t="str">
-        <f>VLOOKUP(B250,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/6/6f/Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Autodromo_Nazionale_Monza%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
+        <f>VLOOKUP(B250,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f6/Aut%C3%B3dromo_Hermanos_Rodr%C3%ADguez%2C_June_4%2C_2018_SkySat_%28cropped%29.jpg/220px-Aut%C3%B3dromo_Hermanos_Rodr%C3%ADguez%2C_June_4%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="251" spans="1:9" x14ac:dyDescent="0.25">
@@ -8907,11 +8907,11 @@
         <v>71</v>
       </c>
       <c r="H251" t="str">
-        <f>VLOOKUP(B251,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B251,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/bd/Silverstone_Circuit_2020.png/250px-Silverstone_Circuit_2020.png</v>
       </c>
       <c r="I251" t="str">
-        <f>VLOOKUP(B251,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B251,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8d/Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg/220px-Silverstone_Circuit%2C_July_2%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -8938,11 +8938,11 @@
         <v>76</v>
       </c>
       <c r="H252" t="str">
-        <f>VLOOKUP(B252,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B252,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/5/54/Spa-Francorchamps_of_Belgium.svg/260px-Spa-Francorchamps_of_Belgium.svg.png</v>
       </c>
       <c r="I252" t="str">
-        <f>VLOOKUP(B252,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B252,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/77/Circuit_de_Spa-Francorchamps%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg/220px-Circuit_de_Spa-Francorchamps%2C_April_22%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -8969,11 +8969,11 @@
         <v>81</v>
       </c>
       <c r="H253" t="str">
-        <f>VLOOKUP(B253,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B253,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/ec/Suzuka_circuit_map--2005.svg/260px-Suzuka_circuit_map--2005.svg.png</v>
       </c>
       <c r="I253" t="str">
-        <f>VLOOKUP(B253,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B253,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/9/9a/Suzuka_International_Racing_Course%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg/220px-Suzuka_International_Racing_Course%2C_July_10%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
@@ -9000,11 +9000,11 @@
         <v>90</v>
       </c>
       <c r="H254" t="str">
-        <f>VLOOKUP(B254,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B254,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f9/%C3%8Ele_Notre-Dame_%28Circuit_Gilles_Villeneuve%29.svg/280px-%C3%8Ele_Notre-Dame_%28Circuit_Gilles_Villeneuve%29.svg.png</v>
       </c>
       <c r="I254" t="str">
-        <f>VLOOKUP(B254,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B254,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/3/38/F1_1978_circuit_ile_notre_dame.png/220px-F1_1978_circuit_ile_notre_dame.png</v>
       </c>
     </row>
@@ -9031,12 +9031,12 @@
         <v>95</v>
       </c>
       <c r="H255" t="str">
-        <f>VLOOKUP(B255,Hoja2!$A$1:$H$35,7)</f>
-        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/4c/Losail.svg/250px-Losail.svg.png</v>
+        <f>VLOOKUP(B255,Hoja2!$A$1:$H$35,7,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/b/b0/Yas_Marina_Circuit.png/250px-Yas_Marina_Circuit.png</v>
       </c>
       <c r="I255" t="str">
-        <f>VLOOKUP(B255,Hoja2!$A$1:$H$35,8)</f>
-        <v>https://www.racefans.net/wp-content/uploads/2021/07/racefansdotnet-21-07-24-21-06-40-1.jpg</v>
+        <f>VLOOKUP(B255,Hoja2!$A$1:$H$35,8,FALSE)</f>
+        <v>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e1/Yas_Marina_Circuit%2C_October_12%2C_2018_SkySat_%28cropped%29.jpg/220px-Yas_Marina_Circuit%2C_October_12%2C_2018_SkySat_%28cropped%29.jpg</v>
       </c>
     </row>
     <row r="256" spans="1:9" x14ac:dyDescent="0.25">
@@ -9062,11 +9062,11 @@
         <v>167</v>
       </c>
       <c r="H256" t="str">
-        <f>VLOOKUP(B256,Hoja2!$A$1:$H$35,7)</f>
+        <f>VLOOKUP(B256,Hoja2!$A$1:$H$35,7,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/7/78/Zandvoort_Circuit.png/250px-Zandvoort_Circuit.png</v>
       </c>
       <c r="I256" t="str">
-        <f>VLOOKUP(B256,Hoja2!$A$1:$H$35,8)</f>
+        <f>VLOOKUP(B256,Hoja2!$A$1:$H$35,8,FALSE)</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/49/Circuit_Park_Zandvoort_from_air_2016-08-24.jpg/220px-Circuit_Park_Zandvoort_from_air_2016-08-24.jpg</v>
       </c>
     </row>

</xml_diff>